<commit_message>
Fix for probe output and reestablishment of D3Q19
</commit_message>
<xml_diff>
--- a/LUMA/tools/spreadsheets/SizingGuide.xlsx
+++ b/LUMA/tools/spreadsheets/SizingGuide.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (CFDTM)\0. Work\3. LBM\C++ Projects\LUMA\LUMA\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (CFDTM)\0. Work\3. LBM\C++ Projects\LUMA\LUMA\tools\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" tabRatio="573" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372" tabRatio="573"/>
   </bookViews>
   <sheets>
     <sheet name="Archer" sheetId="11" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="Desktop" sheetId="7" r:id="rId5"/>
     <sheet name="Laptop" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="69">
   <si>
     <t>No of Nodes</t>
   </si>
@@ -109,9 +109,6 @@
 /Core</t>
   </si>
   <si>
-    <t>Grids = 0</t>
-  </si>
-  <si>
     <t>startx</t>
   </si>
   <si>
@@ -121,33 +118,12 @@
     <t>length</t>
   </si>
   <si>
-    <t>refXstart</t>
-  </si>
-  <si>
-    <t>refXend</t>
-  </si>
-  <si>
-    <t>refYstart</t>
-  </si>
-  <si>
-    <t>refYend</t>
-  </si>
-  <si>
-    <t>Grids = 1</t>
-  </si>
-  <si>
-    <t>Alpha</t>
-  </si>
-  <si>
     <t>N1</t>
   </si>
   <si>
     <t>M1</t>
   </si>
   <si>
-    <t>Grids = 2</t>
-  </si>
-  <si>
     <t>refXstart1</t>
   </si>
   <si>
@@ -181,12 +157,6 @@
     <t>K1</t>
   </si>
   <si>
-    <t>refZstart</t>
-  </si>
-  <si>
-    <t>refZend</t>
-  </si>
-  <si>
     <t>refZstart1</t>
   </si>
   <si>
@@ -205,9 +175,6 @@
     <t>centrez</t>
   </si>
   <si>
-    <t>3D Aerofoil Cases AR = 2</t>
-  </si>
-  <si>
     <t>3D Car</t>
   </si>
   <si>
@@ -271,8 +238,7 @@
     <t>Total Car</t>
   </si>
   <si>
-    <t>Points 
-per L</t>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -292,6 +258,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -366,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -396,6 +363,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -811,10 +781,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -897,32 +867,32 @@
         <v>96</v>
       </c>
       <c r="F2" s="5">
-        <f t="shared" ref="F2:F16" si="2">($C$24/A2)+2</f>
-        <v>12</v>
+        <f t="shared" ref="F2:F16" si="2">($C$23/A2)+2</f>
+        <v>11</v>
       </c>
       <c r="G2" s="5">
-        <f t="shared" ref="G2:G16" si="3">($C$25/B2)+2</f>
-        <v>22</v>
+        <f t="shared" ref="G2:G16" si="3">($C$24/B2)+2</f>
+        <v>38</v>
       </c>
       <c r="H2" s="5">
-        <f t="shared" ref="H2:H16" si="4">($C$26/C2)+2</f>
-        <v>12</v>
+        <f t="shared" ref="H2:H16" si="4">($C$25/C2)+2</f>
+        <v>14</v>
       </c>
       <c r="I2" s="5">
         <f t="shared" ref="I2:I16" si="5">F2*G2*H2</f>
-        <v>3168</v>
+        <v>5852</v>
       </c>
       <c r="J2" s="5">
         <f t="shared" ref="J2:J16" si="6">4*F2*G2+4*G2*H2+4*F2*H2</f>
-        <v>2688</v>
+        <v>4416</v>
       </c>
       <c r="K2" s="5">
         <f t="shared" ref="K2:K16" si="7">J2*E2</f>
-        <v>258048</v>
+        <v>423936</v>
       </c>
       <c r="L2" s="5">
-        <f t="shared" ref="L2:L16" si="8">K2/$C$27*100</f>
-        <v>134.4</v>
+        <f t="shared" ref="L2:L16" si="8">K2/$C$26*100</f>
+        <v>113.58024691358024</v>
       </c>
       <c r="M2" s="6" t="b">
         <f>IF((F2-FLOOR(F2,1))=0,IF((G2-FLOOR(G2,1))=0,IF((H2-FLOOR(H2,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -953,31 +923,31 @@
       </c>
       <c r="F3" s="5">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G3" s="5">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H3" s="5">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I3" s="5">
         <f t="shared" si="5"/>
-        <v>5808</v>
+        <v>10400</v>
       </c>
       <c r="J3" s="5">
         <f t="shared" si="6"/>
-        <v>4048</v>
+        <v>5760</v>
       </c>
       <c r="K3" s="5">
         <f t="shared" si="7"/>
-        <v>194304</v>
+        <v>276480</v>
       </c>
       <c r="L3" s="5">
         <f t="shared" si="8"/>
-        <v>101.2</v>
+        <v>74.074074074074076</v>
       </c>
       <c r="M3" s="6" t="b">
         <f>IF((F3-FLOOR(F3,1))=0,IF((G3-FLOOR(G3,1))=0,IF((H3-FLOOR(H3,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -993,10 +963,10 @@
         <v>4</v>
       </c>
       <c r="B4" s="4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4">
         <v>2</v>
-      </c>
-      <c r="C4" s="4">
-        <v>3</v>
       </c>
       <c r="D4" s="5">
         <f t="shared" si="0"/>
@@ -1008,31 +978,31 @@
       </c>
       <c r="F4" s="5">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G4" s="5">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" si="4"/>
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="I4" s="5">
         <f t="shared" si="5"/>
-        <v>10648</v>
+        <v>19760</v>
       </c>
       <c r="J4" s="5">
         <f t="shared" si="6"/>
-        <v>5808</v>
+        <v>9072</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" si="7"/>
-        <v>139392</v>
+        <v>217728</v>
       </c>
       <c r="L4" s="5">
         <f t="shared" si="8"/>
-        <v>72.599999999999994</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="M4" s="6" t="b">
         <f t="shared" ref="M4:M6" si="10">IF((F4-FLOOR(F4,1))=0,IF((G4-FLOOR(G4,1))=0,IF((H4-FLOOR(H4,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -1045,49 +1015,49 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="4">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" s="4">
         <v>6</v>
       </c>
       <c r="D5" s="5">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" si="1"/>
-        <v>480</v>
+        <v>216</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G5" s="5">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="H5" s="5">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I5" s="5">
         <f t="shared" si="5"/>
-        <v>864</v>
+        <v>2744</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" si="6"/>
-        <v>1152</v>
+        <v>2352</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" si="7"/>
-        <v>552960</v>
+        <v>508032</v>
       </c>
       <c r="L5" s="5">
         <f t="shared" si="8"/>
-        <v>288</v>
+        <v>136.11111111111111</v>
       </c>
       <c r="M5" s="6" t="b">
         <f t="shared" si="10"/>
@@ -1100,49 +1070,49 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B6" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" s="4">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D6" s="5">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" si="1"/>
-        <v>1200</v>
+        <v>432</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="I6" s="5">
         <f t="shared" si="5"/>
-        <v>432</v>
+        <v>1568</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="6"/>
-        <v>720</v>
+        <v>1680</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="7"/>
-        <v>864000</v>
+        <v>725760</v>
       </c>
       <c r="L6" s="5">
         <f t="shared" si="8"/>
-        <v>450</v>
+        <v>194.44444444444443</v>
       </c>
       <c r="M6" s="6" t="b">
         <f t="shared" si="10"/>
@@ -1155,49 +1125,49 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="4">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" s="4">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D7" s="5">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" si="1"/>
-        <v>1440</v>
+        <v>600</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="2"/>
-        <v>8.6666666666666679</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="3"/>
-        <v>5.3333333333333339</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="I7" s="5">
         <f t="shared" si="5"/>
-        <v>369.77777777777789</v>
+        <v>1184.9599999999998</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="6"/>
-        <v>632.88888888888903</v>
+        <v>1368.9599999999998</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="7"/>
-        <v>911360.00000000023</v>
+        <v>821375.99999999988</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" si="8"/>
-        <v>474.6666666666668</v>
+        <v>220.06172839506172</v>
       </c>
       <c r="M7" s="6" t="b">
         <f>IF((F7-FLOOR(F7,1))=0,IF((G7-FLOOR(G7,1))=0,IF((H7-FLOOR(H7,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -1228,31 +1198,31 @@
       </c>
       <c r="F8" s="5">
         <f t="shared" si="2"/>
-        <v>8.6666666666666679</v>
+        <v>8</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="I8" s="5">
         <f t="shared" si="5"/>
-        <v>1664.0000000000002</v>
+        <v>2796.7999999999997</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" si="6"/>
-        <v>2085.3333333333335</v>
+        <v>2908.7999999999997</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" si="7"/>
-        <v>500480.00000000006</v>
+        <v>698111.99999999988</v>
       </c>
       <c r="L8" s="5">
         <f t="shared" si="8"/>
-        <v>260.66666666666669</v>
+        <v>187.03703703703701</v>
       </c>
       <c r="M8" s="6" t="b">
         <f t="shared" ref="M8:M16" si="11">IF((F8-FLOOR(F8,1))=0,IF((G8-FLOOR(G8,1))=0,IF((H8-FLOOR(H8,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -1283,35 +1253,35 @@
       </c>
       <c r="F9" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" si="5"/>
-        <v>2040</v>
+        <v>3607.9999999999995</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="6"/>
-        <v>1976</v>
+        <v>2913.6</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" si="7"/>
-        <v>316160</v>
+        <v>466176</v>
       </c>
       <c r="L9" s="5">
         <f t="shared" si="8"/>
-        <v>164.66666666666669</v>
+        <v>124.89711934156378</v>
       </c>
       <c r="M9" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1338,35 +1308,35 @@
       </c>
       <c r="F10" s="5">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" si="5"/>
-        <v>2040</v>
+        <v>3680</v>
       </c>
       <c r="J10" s="5">
         <f t="shared" si="6"/>
-        <v>1976</v>
+        <v>3072</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" si="7"/>
-        <v>316160</v>
+        <v>491520</v>
       </c>
       <c r="L10" s="5">
         <f t="shared" si="8"/>
-        <v>164.66666666666669</v>
+        <v>131.68724279835391</v>
       </c>
       <c r="M10" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1393,35 +1363,35 @@
       </c>
       <c r="F11" s="5">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6.5</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" si="5"/>
-        <v>2240</v>
+        <v>4050.7999999999997</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" si="6"/>
-        <v>2456</v>
+        <v>3907.2</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="7"/>
-        <v>392960</v>
+        <v>625152</v>
       </c>
       <c r="L11" s="5">
         <f t="shared" si="8"/>
-        <v>204.66666666666669</v>
+        <v>167.48971193415639</v>
       </c>
       <c r="M11" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1448,31 +1418,31 @@
       </c>
       <c r="F12" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" si="5"/>
-        <v>1008</v>
+        <v>1694</v>
       </c>
       <c r="J12" s="5">
         <f t="shared" si="6"/>
-        <v>1248</v>
+        <v>1716</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" si="7"/>
-        <v>479232</v>
+        <v>658944</v>
       </c>
       <c r="L12" s="5">
         <f t="shared" si="8"/>
-        <v>249.6</v>
+        <v>176.54320987654322</v>
       </c>
       <c r="M12" s="6" t="b">
         <f t="shared" si="11"/>
@@ -1503,35 +1473,35 @@
       </c>
       <c r="F13" s="5">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6.5</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I13" s="5">
         <f t="shared" si="5"/>
-        <v>1428</v>
+        <v>2600</v>
       </c>
       <c r="J13" s="5">
         <f t="shared" si="6"/>
-        <v>1628</v>
+        <v>2640</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" si="7"/>
-        <v>416768</v>
+        <v>675840</v>
       </c>
       <c r="L13" s="5">
         <f t="shared" si="8"/>
-        <v>217.06666666666666</v>
+        <v>181.06995884773661</v>
       </c>
       <c r="M13" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N13" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1558,31 +1528,31 @@
       </c>
       <c r="F14" s="5">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H14" s="5">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" si="5"/>
-        <v>1428</v>
+        <v>2420</v>
       </c>
       <c r="J14" s="5">
         <f t="shared" si="6"/>
-        <v>1628</v>
+        <v>2244</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="7"/>
-        <v>416768</v>
+        <v>574464</v>
       </c>
       <c r="L14" s="5">
         <f t="shared" si="8"/>
-        <v>217.06666666666666</v>
+        <v>153.90946502057614</v>
       </c>
       <c r="M14" s="6" t="b">
         <f t="shared" si="11"/>
@@ -1613,35 +1583,35 @@
       </c>
       <c r="F15" s="5">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6.5</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="H15" s="5">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="I15" s="5">
         <f t="shared" si="5"/>
-        <v>1344</v>
+        <v>2272.4</v>
       </c>
       <c r="J15" s="5">
         <f t="shared" si="6"/>
-        <v>1832</v>
+        <v>2625.6</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" si="7"/>
-        <v>586240</v>
+        <v>840192</v>
       </c>
       <c r="L15" s="5">
         <f t="shared" si="8"/>
-        <v>305.33333333333331</v>
+        <v>225.10288065843622</v>
       </c>
       <c r="M15" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N15" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1668,35 +1638,35 @@
       </c>
       <c r="F16" s="5">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I16" s="5">
         <f t="shared" si="5"/>
-        <v>1190</v>
+        <v>2023.9999999999998</v>
       </c>
       <c r="J16" s="5">
         <f t="shared" si="6"/>
-        <v>1436</v>
+        <v>2020.8</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="7"/>
-        <v>459520</v>
+        <v>646656</v>
       </c>
       <c r="L16" s="5">
         <f t="shared" si="8"/>
-        <v>239.33333333333334</v>
+        <v>173.25102880658437</v>
       </c>
       <c r="M16" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N16" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1716,722 +1686,498 @@
     </row>
     <row r="20" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B20" s="14">
-        <v>10</v>
+        <v>1.5</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F20" t="s">
-        <v>57</v>
-      </c>
-      <c r="M20" t="s">
-        <v>58</v>
-      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="14">
-        <v>90</v>
-      </c>
-      <c r="F21" t="s">
-        <v>25</v>
-      </c>
-      <c r="H21" t="s">
-        <v>33</v>
-      </c>
-      <c r="J21" t="s">
-        <v>37</v>
-      </c>
-      <c r="M21" t="s">
-        <v>77</v>
-      </c>
+      <c r="F21" s="17"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="19"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F22" t="s">
-        <v>26</v>
-      </c>
-      <c r="G22" s="13">
-        <f>0.5*($C$24-$B$20*COS($B$21*PI()/180))</f>
-        <v>40</v>
-      </c>
-      <c r="H22" t="s">
-        <v>29</v>
-      </c>
-      <c r="I22" s="13">
-        <f>$C$24/4</f>
-        <v>20</v>
-      </c>
-      <c r="J22" t="s">
-        <v>38</v>
-      </c>
-      <c r="K22" s="13">
-        <f>$C$24/4</f>
-        <v>20</v>
-      </c>
-      <c r="M22" t="s">
-        <v>38</v>
-      </c>
-      <c r="N22" s="16">
-        <f>0.25*(B24-4)*B20</f>
-        <v>10</v>
-      </c>
+      <c r="A22" s="1"/>
+      <c r="B22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="17"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="19"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" t="s">
-        <v>27</v>
-      </c>
-      <c r="G23" s="13">
-        <f>0.5*($C$24-$B$20*SIN($B$21*PI()/180))</f>
-        <v>35</v>
-      </c>
-      <c r="H23" t="s">
-        <v>30</v>
-      </c>
-      <c r="I23" s="13">
-        <f>3*$C$24/4</f>
-        <v>60</v>
-      </c>
-      <c r="J23" t="s">
-        <v>41</v>
-      </c>
-      <c r="K23" s="13">
-        <f>3*$C$24/4</f>
-        <v>60</v>
-      </c>
-      <c r="M23" t="s">
-        <v>41</v>
-      </c>
-      <c r="N23" s="16">
-        <f>N22+(4*B20)</f>
-        <v>50</v>
-      </c>
+      <c r="A23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="15">
+        <v>48</v>
+      </c>
+      <c r="C23" s="3">
+        <f>CEILING($B$20*B23,1)</f>
+        <v>72</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B24" s="15">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="C24" s="3">
-        <f>B20*B24</f>
-        <v>80</v>
+        <f t="shared" ref="C24:C25" si="12">CEILING($B$20*B24,1)</f>
+        <v>72</v>
       </c>
       <c r="E24" s="12"/>
-      <c r="F24" t="s">
-        <v>56</v>
-      </c>
-      <c r="G24" s="13">
-        <f>C26/2</f>
-        <v>30</v>
-      </c>
-      <c r="H24" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="I24" s="13">
-        <f>$C$25/4</f>
-        <v>10</v>
-      </c>
-      <c r="J24" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="K24" s="13">
-        <f>$C$25/4</f>
-        <v>10</v>
-      </c>
-      <c r="M24" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="N24" s="16">
-        <v>0</v>
-      </c>
+      <c r="F24" s="17"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B25" s="15">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="C25" s="3">
-        <f>B20*B25</f>
-        <v>40</v>
-      </c>
-      <c r="E25" s="12"/>
-      <c r="F25" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" s="12">
-        <f>B20*COS(B21*PI()/180)</f>
-        <v>6.1257422745431001E-16</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="I25" s="13">
-        <f>3*$C$25/4</f>
-        <v>30</v>
-      </c>
-      <c r="J25" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="K25" s="13">
-        <f>3*$C$25/4</f>
-        <v>30</v>
-      </c>
-      <c r="M25" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="N25" s="16">
-        <f>1.5*B20</f>
-        <v>15</v>
-      </c>
+        <f t="shared" si="12"/>
+        <v>72</v>
+      </c>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="15">
-        <v>6</v>
+      <c r="B26" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C26" s="3">
-        <f>B20*B26</f>
-        <v>60</v>
-      </c>
-      <c r="H26" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="I26">
-        <f>(($B$26-6)/2)*$B$20</f>
-        <v>0</v>
-      </c>
-      <c r="J26" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="K26">
-        <f>(($B$26-6)/2)*$B$20</f>
-        <v>0</v>
-      </c>
-      <c r="M26" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="N26" s="16">
-        <f>(B26/2-1.5)*B20</f>
-        <v>15</v>
-      </c>
+        <f>C23*C24*C25</f>
+        <v>373248</v>
+      </c>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="3">
-        <f>C24*C25*C26</f>
-        <v>192000</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="I27">
-        <f>$I$26+6*$B$20</f>
-        <v>60</v>
-      </c>
-      <c r="J27" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="K27">
-        <f>$I$26+6*$B$20</f>
-        <v>60</v>
-      </c>
-      <c r="M27" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="N27" s="16">
-        <f>N26+(3*B20)</f>
-        <v>45</v>
-      </c>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="19"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H28" t="s">
-        <v>35</v>
-      </c>
-      <c r="I28" s="13">
-        <f>($I$23-$I$22+1)*2</f>
-        <v>82</v>
-      </c>
-      <c r="J28" t="s">
-        <v>35</v>
-      </c>
-      <c r="K28" s="13">
-        <f>($I$23-$I$22+1)*2</f>
-        <v>82</v>
-      </c>
-      <c r="M28" t="s">
-        <v>35</v>
-      </c>
-      <c r="N28" s="12">
-        <f>(N23-N22+1)*2</f>
-        <v>82</v>
-      </c>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>78</v>
-      </c>
-      <c r="C29" s="13">
-        <f>(C24*C25*C26)+ (N28*N29*N30) + (N37*N38*N39) + (N46*N47*N48) + (N55*N56*N57)</f>
-        <v>12063952</v>
-      </c>
-      <c r="H29" t="s">
-        <v>36</v>
-      </c>
-      <c r="I29" s="13">
-        <f>($I$25-$I$24+1)*2</f>
-        <v>42</v>
-      </c>
-      <c r="J29" t="s">
-        <v>36</v>
-      </c>
-      <c r="K29" s="13">
-        <f>($I$25-$I$24+1)*2</f>
-        <v>42</v>
-      </c>
-      <c r="M29" t="s">
-        <v>36</v>
-      </c>
-      <c r="N29" s="12">
-        <f>(N25-N24+1)*2</f>
-        <v>32</v>
-      </c>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="19"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H30" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="I30" s="13">
-        <f>($I$27-$I$26+1)*2</f>
-        <v>122</v>
-      </c>
-      <c r="J30" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="K30">
-        <f>($I$27-$I$26+1)*2</f>
-        <v>122</v>
-      </c>
-      <c r="M30" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="N30" s="12">
-        <f>(N27-N26+1)*2</f>
-        <v>62</v>
-      </c>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="19"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H31" t="s">
-        <v>26</v>
-      </c>
-      <c r="I31" s="13">
-        <f>0.5*($I$28-$B$20*2*COS($B$21*PI()/180))</f>
-        <v>41</v>
-      </c>
-      <c r="J31" t="s">
-        <v>43</v>
-      </c>
-      <c r="K31" s="13">
-        <f>($K$28/4)</f>
-        <v>20.5</v>
-      </c>
-      <c r="M31" t="s">
-        <v>43</v>
-      </c>
-      <c r="N31" s="16">
-        <f>(B20/4)*2</f>
-        <v>5</v>
-      </c>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H32" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="I32" s="13">
-        <f>0.5*($I$28-$B$20*2*SIN($B$21*PI()/180))</f>
-        <v>31</v>
-      </c>
-      <c r="J32" t="s">
-        <v>39</v>
-      </c>
-      <c r="K32" s="13">
-        <f>(3*$K$28/4)</f>
-        <v>61.5</v>
-      </c>
-      <c r="M32" t="s">
-        <v>39</v>
-      </c>
-      <c r="N32" s="16">
-        <f>N31+(3.25*B20*2)</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H33" t="s">
-        <v>56</v>
-      </c>
-      <c r="I33" s="13">
-        <f>I30/2</f>
-        <v>61</v>
-      </c>
-      <c r="J33" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="K33" s="13">
-        <f>($K$29/4)</f>
-        <v>10.5</v>
-      </c>
-      <c r="M33" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="N33" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H34" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I34" s="13">
-        <f>$B$20*2*COS($B$21*PI()/180)</f>
-        <v>1.22514845490862E-15</v>
-      </c>
-      <c r="J34" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K34" s="13">
-        <f>(3*$K$29/4)</f>
-        <v>31.5</v>
-      </c>
-      <c r="M34" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="N34" s="16">
-        <f>N33+(1.25*B20*2)</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H35" s="12"/>
-      <c r="J35" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="K35">
-        <f>$B$20*2</f>
-        <v>20</v>
-      </c>
-      <c r="M35" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="N35" s="16">
-        <f>(B20/4)*2</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="J36" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="K36">
-        <f>K35+(5*B20*2)</f>
-        <v>120</v>
-      </c>
-      <c r="M36" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="N36" s="16">
-        <f>N35+(2.5*B20*2)</f>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="J37" t="s">
-        <v>46</v>
-      </c>
-      <c r="K37" s="13">
-        <f>($K$32-$K$31+1)*2</f>
-        <v>84</v>
-      </c>
-      <c r="M37" t="s">
-        <v>46</v>
-      </c>
-      <c r="N37" s="12">
-        <f>(N32-N31+1)*2</f>
-        <v>132</v>
-      </c>
-    </row>
-    <row r="38" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="J38" t="s">
-        <v>47</v>
-      </c>
-      <c r="K38" s="13">
-        <f>($K$34-$K$33+1)*2</f>
-        <v>44</v>
-      </c>
-      <c r="M38" t="s">
-        <v>47</v>
-      </c>
-      <c r="N38" s="12">
-        <f>(N34-N33+1)*2</f>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="J39" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="K39" s="13">
-        <f>($K$36-$K$35+1)*2</f>
-        <v>202</v>
-      </c>
-      <c r="M39" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="N39" s="12">
-        <f>(N36-N35+1)*2</f>
-        <v>102</v>
-      </c>
-    </row>
-    <row r="40" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="J40" t="s">
-        <v>26</v>
-      </c>
-      <c r="K40" s="13">
-        <f>0.5*($K$37-$B$20*4*COS($B$21*PI()/180))</f>
-        <v>42</v>
-      </c>
-      <c r="M40" t="s">
-        <v>59</v>
-      </c>
-      <c r="N40" s="16">
-        <f>(B20/4)*4</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="J41" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="K41" s="13">
-        <f>0.5*($K$38-$B$20*4*SIN($B$21*PI()/180))</f>
-        <v>2</v>
-      </c>
-      <c r="M41" t="s">
-        <v>60</v>
-      </c>
-      <c r="N41" s="16">
-        <f>N40+(2.5*B20*4)</f>
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="J42" t="s">
-        <v>56</v>
-      </c>
-      <c r="K42" s="13">
-        <f>K39/2</f>
-        <v>101</v>
-      </c>
-      <c r="M42" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="N42" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="J43" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K43" s="13">
-        <f>$B$20*4*COS($B$21*PI()/180)</f>
-        <v>2.45029690981724E-15</v>
-      </c>
-      <c r="M43" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="N43" s="16">
-        <f>B20*4</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="M44" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="N44" s="16">
-        <f>(B20/4)*4</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="M45" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="N45" s="16">
-        <f>N44+(2*B20*4)</f>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="46" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="M46" t="s">
-        <v>65</v>
-      </c>
-      <c r="N46" s="12">
-        <f>(N41-N40+1)*2</f>
-        <v>202</v>
-      </c>
-    </row>
-    <row r="47" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="M47" t="s">
-        <v>66</v>
-      </c>
-      <c r="N47" s="12">
-        <f>(N43-N42+1)*2</f>
-        <v>82</v>
-      </c>
-    </row>
-    <row r="48" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="M48" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="N48" s="12">
-        <f>(N45-N44+1)*2</f>
-        <v>162</v>
-      </c>
-    </row>
-    <row r="49" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M49" t="s">
-        <v>68</v>
-      </c>
-      <c r="N49" s="16">
-        <f>(B20/4)*8</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M50" t="s">
-        <v>69</v>
-      </c>
-      <c r="N50" s="16">
-        <f>N49+(1.75*B20*8)</f>
-        <v>160</v>
-      </c>
-    </row>
-    <row r="51" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M51" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="N51" s="16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M52" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="N52" s="16">
-        <f>0.75*B20*8</f>
-        <v>60</v>
-      </c>
-    </row>
-    <row r="53" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M53" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="N53" s="16">
-        <f>(B20/4)*8</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="54" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M54" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="N54" s="16">
-        <f>N53+(1.5*B20*8)</f>
-        <v>140</v>
-      </c>
-    </row>
-    <row r="55" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M55" t="s">
-        <v>74</v>
-      </c>
-      <c r="N55" s="12">
-        <f>(N50-N49+1)*2</f>
-        <v>282</v>
-      </c>
-    </row>
-    <row r="56" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M56" t="s">
-        <v>76</v>
-      </c>
-      <c r="N56" s="12">
-        <f>(N52-N51+1)*2</f>
-        <v>122</v>
-      </c>
-    </row>
-    <row r="57" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M57" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="N57" s="12">
-        <f>(N54-N53+1)*2</f>
-        <v>242</v>
-      </c>
-    </row>
-    <row r="58" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M58" t="s">
-        <v>26</v>
-      </c>
-      <c r="N58" s="16">
-        <f>(B20/4)*16</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="59" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M59" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="N59" s="16">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="60" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M60" t="s">
-        <v>56</v>
-      </c>
-      <c r="N60" s="16">
-        <f>N57/2</f>
-        <v>121</v>
-      </c>
-    </row>
-    <row r="61" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M61" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="N61" s="16">
-        <f>B20*16</f>
-        <v>160</v>
-      </c>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+    </row>
+    <row r="33" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+    </row>
+    <row r="34" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+    </row>
+    <row r="35" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="19"/>
+    </row>
+    <row r="36" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="19"/>
+    </row>
+    <row r="37" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+    </row>
+    <row r="38" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="19"/>
+    </row>
+    <row r="39" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="19"/>
+    </row>
+    <row r="40" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+    </row>
+    <row r="41" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="19"/>
+    </row>
+    <row r="42" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="19"/>
+    </row>
+    <row r="43" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="17"/>
+      <c r="L43" s="17"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="19"/>
+    </row>
+    <row r="44" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="17"/>
+      <c r="L44" s="17"/>
+      <c r="M44" s="17"/>
+      <c r="N44" s="19"/>
+    </row>
+    <row r="45" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F45" s="17"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="17"/>
+      <c r="K45" s="17"/>
+      <c r="L45" s="17"/>
+      <c r="M45" s="17"/>
+      <c r="N45" s="19"/>
+    </row>
+    <row r="46" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
+      <c r="M46" s="19"/>
+      <c r="N46" s="19"/>
+    </row>
+    <row r="47" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="17"/>
+      <c r="L47" s="17"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="19"/>
+    </row>
+    <row r="48" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F48" s="17"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="17"/>
+      <c r="L48" s="17"/>
+      <c r="M48" s="17"/>
+      <c r="N48" s="19"/>
+    </row>
+    <row r="49" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="17"/>
+      <c r="J49" s="17"/>
+      <c r="K49" s="17"/>
+      <c r="L49" s="17"/>
+      <c r="M49" s="19"/>
+      <c r="N49" s="19"/>
+    </row>
+    <row r="50" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="17"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="19"/>
+    </row>
+    <row r="51" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="17"/>
+      <c r="J51" s="17"/>
+      <c r="K51" s="17"/>
+      <c r="L51" s="17"/>
+      <c r="M51" s="19"/>
+      <c r="N51" s="19"/>
+    </row>
+    <row r="52" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="17"/>
+      <c r="K52" s="17"/>
+      <c r="L52" s="17"/>
+      <c r="M52" s="19"/>
+      <c r="N52" s="19"/>
+    </row>
+    <row r="53" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F53" s="17"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="17"/>
+      <c r="L53" s="17"/>
+      <c r="M53" s="17"/>
+      <c r="N53" s="19"/>
+    </row>
+    <row r="54" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F54" s="17"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="17"/>
+      <c r="J54" s="17"/>
+      <c r="K54" s="17"/>
+      <c r="L54" s="17"/>
+      <c r="M54" s="17"/>
+      <c r="N54" s="19"/>
+    </row>
+    <row r="55" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F55" s="17"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="17"/>
+      <c r="J55" s="17"/>
+      <c r="K55" s="17"/>
+      <c r="L55" s="17"/>
+      <c r="M55" s="19"/>
+      <c r="N55" s="19"/>
+    </row>
+    <row r="56" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="17"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17"/>
+      <c r="N56" s="19"/>
+    </row>
+    <row r="57" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
+      <c r="I57" s="17"/>
+      <c r="J57" s="17"/>
+      <c r="K57" s="17"/>
+      <c r="L57" s="17"/>
+      <c r="M57" s="19"/>
+      <c r="N57" s="19"/>
+    </row>
+    <row r="58" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F58" s="17"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+      <c r="J58" s="17"/>
+      <c r="K58" s="17"/>
+      <c r="L58" s="17"/>
+      <c r="M58" s="17"/>
+      <c r="N58" s="19"/>
+    </row>
+    <row r="59" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+      <c r="J59" s="17"/>
+      <c r="K59" s="17"/>
+      <c r="L59" s="17"/>
+      <c r="M59" s="19"/>
+      <c r="N59" s="19"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:N16">
@@ -2456,8 +2202,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3359,7 +3105,7 @@
     </row>
     <row r="20" spans="1:14" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="B20">
         <v>10</v>
@@ -3368,17 +3114,17 @@
         <v>18</v>
       </c>
       <c r="M20" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M21" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M22" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="N22" s="16">
         <f>0.25*(B24-4)*B20</f>
@@ -3394,7 +3140,7 @@
         <v>12</v>
       </c>
       <c r="M23" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="N23" s="16">
         <f>N22+(4*B20)</f>
@@ -3416,7 +3162,7 @@
       <c r="H24" s="12"/>
       <c r="J24" s="12"/>
       <c r="M24" s="12" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="N24" s="16">
         <v>0</v>
@@ -3437,7 +3183,7 @@
       <c r="H25" s="12"/>
       <c r="J25" s="12"/>
       <c r="M25" s="12" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N25" s="16">
         <f>1.5*B20</f>
@@ -3457,7 +3203,7 @@
       </c>
       <c r="J26" s="12"/>
       <c r="M26" s="12" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="N26" s="16">
         <f>((B26/2-1.5)*B20) - 1</f>
@@ -3475,7 +3221,7 @@
       <c r="H27" s="12"/>
       <c r="J27" s="12"/>
       <c r="M27" s="12" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="N27" s="16">
         <f>N26+(3*B20)</f>
@@ -3486,7 +3232,7 @@
       <c r="H28" s="12"/>
       <c r="J28" s="12"/>
       <c r="M28" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="N28" s="12">
         <f>(N23-N22+1)*2</f>
@@ -3495,7 +3241,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C29" s="13">
         <f>(C24*C25*C26)+ (N28*N29*N30) + (N37*N38*N39) + (N46*N47*N48) + (N55*N56*N57)</f>
@@ -3503,7 +3249,7 @@
       </c>
       <c r="J29" s="12"/>
       <c r="M29" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="N29" s="12">
         <f>(N25-N24+1)*2</f>
@@ -3514,7 +3260,7 @@
       <c r="H30" s="12"/>
       <c r="J30" s="12"/>
       <c r="M30" s="12" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="N30" s="12">
         <f>(N27-N26+1)*2</f>
@@ -3525,7 +3271,7 @@
       <c r="H31" s="12"/>
       <c r="J31" s="12"/>
       <c r="M31" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="N31" s="16">
         <f>(B20/4)*2</f>
@@ -3535,7 +3281,7 @@
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J32" s="12"/>
       <c r="M32" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="N32" s="16">
         <f>N31+(3.25*B20*2)</f>
@@ -3546,7 +3292,7 @@
       <c r="H33" s="12"/>
       <c r="J33" s="12"/>
       <c r="M33" s="12" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="N33" s="16">
         <v>0</v>
@@ -3555,7 +3301,7 @@
     <row r="34" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H34" s="12"/>
       <c r="M34" s="12" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="N34" s="16">
         <f>N33+(1.25*B20*2)</f>
@@ -3564,7 +3310,7 @@
     </row>
     <row r="35" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M35" s="12" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="N35" s="16">
         <f>(B20/4)*2</f>
@@ -3573,7 +3319,7 @@
     </row>
     <row r="36" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M36" s="12" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="N36" s="16">
         <f>N35+(2.5*B20*2)</f>
@@ -3582,7 +3328,7 @@
     </row>
     <row r="37" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M37" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="N37" s="12">
         <f>(N32-N31+1)*2</f>
@@ -3591,7 +3337,7 @@
     </row>
     <row r="38" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M38" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="N38" s="12">
         <f>(N34-N33+1)*2</f>
@@ -3600,7 +3346,7 @@
     </row>
     <row r="39" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M39" s="12" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="N39" s="12">
         <f>(N36-N35+1)*2</f>
@@ -3609,7 +3355,7 @@
     </row>
     <row r="40" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M40" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="N40" s="16">
         <f>(B20/4)*4</f>
@@ -3618,7 +3364,7 @@
     </row>
     <row r="41" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M41" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="N41" s="16">
         <f>N40+(2.5*B20*4)</f>
@@ -3627,7 +3373,7 @@
     </row>
     <row r="42" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M42" s="12" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="N42" s="16">
         <v>0</v>
@@ -3635,7 +3381,7 @@
     </row>
     <row r="43" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M43" s="12" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="N43" s="16">
         <f>B20*4</f>
@@ -3644,7 +3390,7 @@
     </row>
     <row r="44" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M44" s="12" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="N44" s="16">
         <f>(B20/4)*4</f>
@@ -3653,7 +3399,7 @@
     </row>
     <row r="45" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M45" s="12" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="N45" s="16">
         <f>N44+(2*B20*4)</f>
@@ -3662,7 +3408,7 @@
     </row>
     <row r="46" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M46" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="N46" s="12">
         <f>(N41-N40+1)*2</f>
@@ -3671,7 +3417,7 @@
     </row>
     <row r="47" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M47" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="N47" s="12">
         <f>(N43-N42+1)*2</f>
@@ -3680,7 +3426,7 @@
     </row>
     <row r="48" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M48" s="12" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="N48" s="12">
         <f>(N45-N44+1)*2</f>
@@ -3689,7 +3435,7 @@
     </row>
     <row r="49" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M49" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="N49" s="16">
         <f>(B20/4)*8</f>
@@ -3698,7 +3444,7 @@
     </row>
     <row r="50" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M50" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="N50" s="16">
         <f>N49+(1.75*B20*8)</f>
@@ -3707,7 +3453,7 @@
     </row>
     <row r="51" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M51" s="12" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="N51" s="16">
         <v>0</v>
@@ -3715,7 +3461,7 @@
     </row>
     <row r="52" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M52" s="12" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="N52" s="16">
         <f>0.75*B20*8</f>
@@ -3724,7 +3470,7 @@
     </row>
     <row r="53" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M53" s="12" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="N53" s="16">
         <f>(B20/4)*8</f>
@@ -3733,7 +3479,7 @@
     </row>
     <row r="54" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M54" s="12" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="N54" s="16">
         <f>N53+(1.5*B20*8)</f>
@@ -3742,7 +3488,7 @@
     </row>
     <row r="55" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M55" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="N55" s="12">
         <f>(N50-N49+1)*2</f>
@@ -3751,7 +3497,7 @@
     </row>
     <row r="56" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M56" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="N56" s="12">
         <f>(N52-N51+1)*2</f>
@@ -3760,7 +3506,7 @@
     </row>
     <row r="57" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M57" s="12" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="N57" s="12">
         <f>(N54-N53+1)*2</f>
@@ -3769,7 +3515,7 @@
     </row>
     <row r="58" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M58" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N58" s="16">
         <f>(B20/4)*16</f>
@@ -3778,7 +3524,7 @@
     </row>
     <row r="59" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M59" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N59" s="16">
         <v>16</v>
@@ -3786,7 +3532,7 @@
     </row>
     <row r="60" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M60" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="N60" s="16">
         <f>N57/2</f>
@@ -3795,7 +3541,7 @@
     </row>
     <row r="61" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M61" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N61" s="16">
         <f>B20*16</f>
@@ -6395,17 +6141,17 @@
         <v>18</v>
       </c>
       <c r="M7" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M8" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M9" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="N9" s="16">
         <f>0.25*(B11-4)*B7</f>
@@ -6421,7 +6167,7 @@
         <v>12</v>
       </c>
       <c r="M10" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="N10" s="16">
         <f>N9+(4*B7)</f>
@@ -6443,7 +6189,7 @@
       <c r="H11" s="12"/>
       <c r="J11" s="12"/>
       <c r="M11" s="12" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="N11" s="16">
         <v>0</v>
@@ -6464,7 +6210,7 @@
       <c r="H12" s="12"/>
       <c r="J12" s="12"/>
       <c r="M12" s="12" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N12" s="16">
         <f>1.5*B7</f>
@@ -6484,7 +6230,7 @@
       </c>
       <c r="J13" s="12"/>
       <c r="M13" s="12" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="N13" s="16">
         <f>(B13/2-1.5)*B7</f>
@@ -6502,7 +6248,7 @@
       <c r="H14" s="12"/>
       <c r="J14" s="12"/>
       <c r="M14" s="12" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="N14" s="16">
         <f>N13+(3*B7)</f>
@@ -6513,7 +6259,7 @@
       <c r="H15" s="12"/>
       <c r="J15" s="12"/>
       <c r="M15" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="N15" s="12">
         <f>(N10-N9+1)*2</f>
@@ -6522,7 +6268,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C16" s="13">
         <f>(C11*C12*C13)+ (N15*N16*N17) + (N24*N25*N26) + (N33*N34*N35) + (N42*N43*N44)</f>
@@ -6530,7 +6276,7 @@
       </c>
       <c r="J16" s="12"/>
       <c r="M16" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="N16" s="12">
         <f>(N12-N11+1)*2</f>
@@ -6541,7 +6287,7 @@
       <c r="H17" s="12"/>
       <c r="J17" s="12"/>
       <c r="M17" s="12" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="N17" s="12">
         <f>(N14-N13+1)*2</f>
@@ -6552,7 +6298,7 @@
       <c r="H18" s="12"/>
       <c r="J18" s="12"/>
       <c r="M18" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="N18" s="16">
         <f>(B7/4)*2</f>
@@ -6562,7 +6308,7 @@
     <row r="19" spans="8:14" x14ac:dyDescent="0.25">
       <c r="J19" s="12"/>
       <c r="M19" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="N19" s="16">
         <f>N18+(3.25*B7*2)</f>
@@ -6573,7 +6319,7 @@
       <c r="H20" s="12"/>
       <c r="J20" s="12"/>
       <c r="M20" s="12" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="N20" s="16">
         <v>0</v>
@@ -6582,7 +6328,7 @@
     <row r="21" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H21" s="12"/>
       <c r="M21" s="12" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="N21" s="16">
         <f>N20+(1.25*B7*2)</f>
@@ -6591,7 +6337,7 @@
     </row>
     <row r="22" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M22" s="12" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="N22" s="16">
         <f>(B7/4)*2</f>
@@ -6600,7 +6346,7 @@
     </row>
     <row r="23" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M23" s="12" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="N23" s="16">
         <f>N22+(2.5*B7*2)</f>
@@ -6609,7 +6355,7 @@
     </row>
     <row r="24" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M24" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="N24" s="12">
         <f>(N19-N18+1)*2</f>
@@ -6618,7 +6364,7 @@
     </row>
     <row r="25" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M25" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="N25" s="12">
         <f>(N21-N20+1)*2</f>
@@ -6627,7 +6373,7 @@
     </row>
     <row r="26" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M26" s="12" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="N26" s="12">
         <f>(N23-N22+1)*2</f>
@@ -6636,7 +6382,7 @@
     </row>
     <row r="27" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M27" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="N27" s="16">
         <f>(B7/4)*4</f>
@@ -6645,7 +6391,7 @@
     </row>
     <row r="28" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M28" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="N28" s="16">
         <f>N27+(2.5*B7*4)</f>
@@ -6654,7 +6400,7 @@
     </row>
     <row r="29" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M29" s="12" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="N29" s="16">
         <v>0</v>
@@ -6662,7 +6408,7 @@
     </row>
     <row r="30" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M30" s="12" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="N30" s="16">
         <f>B7*4</f>
@@ -6671,7 +6417,7 @@
     </row>
     <row r="31" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M31" s="12" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="N31" s="16">
         <f>(B7/4)*4</f>
@@ -6680,7 +6426,7 @@
     </row>
     <row r="32" spans="8:14" x14ac:dyDescent="0.25">
       <c r="M32" s="12" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="N32" s="16">
         <f>N31+(2*B7*4)</f>
@@ -6689,7 +6435,7 @@
     </row>
     <row r="33" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M33" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="N33" s="12">
         <f>(N28-N27+1)*2</f>
@@ -6698,7 +6444,7 @@
     </row>
     <row r="34" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M34" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="N34" s="12">
         <f>(N30-N29+1)*2</f>
@@ -6707,7 +6453,7 @@
     </row>
     <row r="35" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M35" s="12" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="N35" s="12">
         <f>(N32-N31+1)*2</f>
@@ -6716,7 +6462,7 @@
     </row>
     <row r="36" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M36" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="N36" s="16">
         <f>(B7/4)*8</f>
@@ -6725,7 +6471,7 @@
     </row>
     <row r="37" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M37" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="N37" s="16">
         <f>N36+(1.75*B7*8)</f>
@@ -6734,7 +6480,7 @@
     </row>
     <row r="38" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M38" s="12" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="N38" s="16">
         <v>0</v>
@@ -6742,7 +6488,7 @@
     </row>
     <row r="39" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M39" s="12" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="N39" s="16">
         <f>0.75*B7*8</f>
@@ -6751,7 +6497,7 @@
     </row>
     <row r="40" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M40" s="12" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="N40" s="16">
         <f>(B7/4)*8</f>
@@ -6760,7 +6506,7 @@
     </row>
     <row r="41" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M41" s="12" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="N41" s="16">
         <f>N40+(1.5*B7*8)</f>
@@ -6769,7 +6515,7 @@
     </row>
     <row r="42" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M42" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="N42" s="12">
         <f>(N37-N36+1)*2</f>
@@ -6778,7 +6524,7 @@
     </row>
     <row r="43" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M43" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="N43" s="12">
         <f>(N39-N38+1)*2</f>
@@ -6787,7 +6533,7 @@
     </row>
     <row r="44" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M44" s="12" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="N44" s="12">
         <f>(N41-N40+1)*2</f>
@@ -6796,7 +6542,7 @@
     </row>
     <row r="45" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N45" s="16">
         <f>(B7/4)*16</f>
@@ -6805,7 +6551,7 @@
     </row>
     <row r="46" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M46" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N46" s="16">
         <v>16</v>
@@ -6813,7 +6559,7 @@
     </row>
     <row r="47" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M47" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="N47" s="16">
         <f>N44/2</f>
@@ -6822,7 +6568,7 @@
     </row>
     <row r="48" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M48" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N48" s="16">
         <f>B7*16</f>

</xml_diff>

<commit_message>
Corrected error in sizing guide plus updated merge tool.
</commit_message>
<xml_diff>
--- a/LUMA/tools/spreadsheets/SizingGuide.xlsx
+++ b/LUMA/tools/spreadsheets/SizingGuide.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (CFDTM)\0. Work\3. LBM\C++ Projects\LUMA\LUMA\tools\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (The University of Manchester)\0. Work\3. LBM\C++ Projects\LUMA\LUMA\tools\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -784,7 +784,7 @@
   <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -850,49 +850,49 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
       </c>
       <c r="C2" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D2" s="5">
         <f t="shared" ref="D2:D16" si="0">E2/$B$19</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E2" s="5">
         <f t="shared" ref="E2:E16" si="1">A2*B2*C2</f>
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="F2" s="5">
         <f t="shared" ref="F2:F16" si="2">($C$23/A2)+2</f>
-        <v>11</v>
+        <v>194</v>
       </c>
       <c r="G2" s="5">
         <f t="shared" ref="G2:G16" si="3">($C$24/B2)+2</f>
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="H2" s="5">
         <f t="shared" ref="H2:H16" si="4">($C$25/C2)+2</f>
-        <v>14</v>
+        <v>98</v>
       </c>
       <c r="I2" s="5">
-        <f t="shared" ref="I2:I16" si="5">F2*G2*H2</f>
-        <v>5852</v>
+        <f>F2*G2*H2</f>
+        <v>1863176</v>
       </c>
       <c r="J2" s="5">
-        <f t="shared" ref="J2:J16" si="6">4*F2*G2+4*G2*H2+4*F2*H2</f>
-        <v>4416</v>
+        <f>((F2*G2) + (G2*(H2-2)) + ((F2-2)*(H2-2)))*2</f>
+        <v>93704</v>
       </c>
       <c r="K2" s="5">
-        <f t="shared" ref="K2:K16" si="7">J2*E2</f>
-        <v>423936</v>
+        <f t="shared" ref="K2:K16" si="5">J2*E2</f>
+        <v>2248896</v>
       </c>
       <c r="L2" s="5">
-        <f t="shared" ref="L2:L16" si="8">K2/$C$26*100</f>
-        <v>113.58024691358024</v>
+        <f t="shared" ref="L2:L16" si="6">K2/$C$26*100</f>
+        <v>5.2955910011574074</v>
       </c>
       <c r="M2" s="6" t="b">
         <f>IF((F2-FLOOR(F2,1))=0,IF((G2-FLOOR(G2,1))=0,IF((H2-FLOOR(H2,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -905,13 +905,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="4">
         <v>4</v>
       </c>
       <c r="C3" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="5">
         <f t="shared" si="0"/>
@@ -923,31 +923,31 @@
       </c>
       <c r="F3" s="5">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>194</v>
       </c>
       <c r="G3" s="5">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="H3" s="5">
         <f t="shared" si="4"/>
-        <v>26</v>
+        <v>98</v>
       </c>
       <c r="I3" s="5">
+        <f t="shared" ref="I2:I16" si="7">F3*G3*H3</f>
+        <v>950600</v>
+      </c>
+      <c r="J3" s="5">
+        <f t="shared" ref="J3:J16" si="8">((F3*G3) + (G3*(H3-2)) + ((F3-2)*(H3-2)))*2</f>
+        <v>65864</v>
+      </c>
+      <c r="K3" s="5">
         <f t="shared" si="5"/>
-        <v>10400</v>
-      </c>
-      <c r="J3" s="5">
+        <v>3161472</v>
+      </c>
+      <c r="L3" s="5">
         <f t="shared" si="6"/>
-        <v>5760</v>
-      </c>
-      <c r="K3" s="5">
-        <f t="shared" si="7"/>
-        <v>276480</v>
-      </c>
-      <c r="L3" s="5">
-        <f t="shared" si="8"/>
-        <v>74.074074074074076</v>
+        <v>7.4444806134259256</v>
       </c>
       <c r="M3" s="6" t="b">
         <f>IF((F3-FLOOR(F3,1))=0,IF((G3-FLOOR(G3,1))=0,IF((H3-FLOOR(H3,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -960,49 +960,49 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4">
         <v>4</v>
       </c>
-      <c r="B4" s="4">
-        <v>3</v>
-      </c>
       <c r="C4" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D4" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E4" s="5">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>194</v>
       </c>
       <c r="G4" s="5">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="I4" s="5">
+        <f t="shared" si="7"/>
+        <v>485000</v>
+      </c>
+      <c r="J4" s="5">
+        <f t="shared" si="8"/>
+        <v>42632</v>
+      </c>
+      <c r="K4" s="5">
         <f t="shared" si="5"/>
-        <v>19760</v>
-      </c>
-      <c r="J4" s="5">
+        <v>4092672</v>
+      </c>
+      <c r="L4" s="5">
         <f t="shared" si="6"/>
-        <v>9072</v>
-      </c>
-      <c r="K4" s="5">
-        <f t="shared" si="7"/>
-        <v>217728</v>
-      </c>
-      <c r="L4" s="5">
-        <f t="shared" si="8"/>
-        <v>58.333333333333336</v>
+        <v>9.6372251157407405</v>
       </c>
       <c r="M4" s="6" t="b">
         <f t="shared" ref="M4:M6" si="10">IF((F4-FLOOR(F4,1))=0,IF((G4-FLOOR(G4,1))=0,IF((H4-FLOOR(H4,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -1015,49 +1015,49 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5" s="5">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="5">
         <f t="shared" si="1"/>
-        <v>216</v>
+        <v>192</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>98</v>
       </c>
       <c r="G5" s="5">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="H5" s="5">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="I5" s="5">
+        <f t="shared" si="7"/>
+        <v>245000</v>
+      </c>
+      <c r="J5" s="5">
+        <f t="shared" si="8"/>
+        <v>23816</v>
+      </c>
+      <c r="K5" s="5">
         <f t="shared" si="5"/>
-        <v>2744</v>
-      </c>
-      <c r="J5" s="5">
+        <v>4572672</v>
+      </c>
+      <c r="L5" s="5">
         <f t="shared" si="6"/>
-        <v>2352</v>
-      </c>
-      <c r="K5" s="5">
-        <f t="shared" si="7"/>
-        <v>508032</v>
-      </c>
-      <c r="L5" s="5">
-        <f t="shared" si="8"/>
-        <v>136.11111111111111</v>
+        <v>10.767505787037036</v>
       </c>
       <c r="M5" s="6" t="b">
         <f t="shared" si="10"/>
@@ -1073,46 +1073,46 @@
         <v>12</v>
       </c>
       <c r="B6" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C6" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D6" s="5">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" s="5">
         <f t="shared" si="1"/>
-        <v>432</v>
+        <v>384</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>98</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="I6" s="5">
+        <f t="shared" si="7"/>
+        <v>127400</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" si="8"/>
+        <v>16808</v>
+      </c>
+      <c r="K6" s="5">
         <f t="shared" si="5"/>
-        <v>1568</v>
-      </c>
-      <c r="J6" s="5">
+        <v>6454272</v>
+      </c>
+      <c r="L6" s="5">
         <f t="shared" si="6"/>
-        <v>1680</v>
-      </c>
-      <c r="K6" s="5">
-        <f t="shared" si="7"/>
-        <v>725760</v>
-      </c>
-      <c r="L6" s="5">
-        <f t="shared" si="8"/>
-        <v>194.44444444444443</v>
+        <v>15.198206018518517</v>
       </c>
       <c r="M6" s="6" t="b">
         <f t="shared" si="10"/>
@@ -1125,53 +1125,53 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D7" s="5">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E7" s="5">
         <f t="shared" si="1"/>
-        <v>600</v>
+        <v>768</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="2"/>
-        <v>9.1999999999999993</v>
+        <v>98</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="3"/>
-        <v>9.1999999999999993</v>
+        <v>26</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="I7" s="5">
+        <f t="shared" si="7"/>
+        <v>66248</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" si="8"/>
+        <v>10952</v>
+      </c>
+      <c r="K7" s="5">
         <f t="shared" si="5"/>
-        <v>1184.9599999999998</v>
-      </c>
-      <c r="J7" s="5">
+        <v>8411136</v>
+      </c>
+      <c r="L7" s="5">
         <f t="shared" si="6"/>
-        <v>1368.9599999999998</v>
-      </c>
-      <c r="K7" s="5">
-        <f t="shared" si="7"/>
-        <v>821375.99999999988</v>
-      </c>
-      <c r="L7" s="5">
-        <f t="shared" si="8"/>
-        <v>220.06172839506172</v>
+        <v>19.80613425925926</v>
       </c>
       <c r="M7" s="6" t="b">
         <f>IF((F7-FLOOR(F7,1))=0,IF((G7-FLOOR(G7,1))=0,IF((H7-FLOOR(H7,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1180,53 +1180,53 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B8" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" s="4">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>64</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="1"/>
-        <v>240</v>
+        <v>1536</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="3"/>
-        <v>9.1999999999999993</v>
+        <v>26</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I8" s="5">
+        <f t="shared" si="7"/>
+        <v>33800</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" si="8"/>
+        <v>6152</v>
+      </c>
+      <c r="K8" s="5">
         <f t="shared" si="5"/>
-        <v>2796.7999999999997</v>
-      </c>
-      <c r="J8" s="5">
+        <v>9449472</v>
+      </c>
+      <c r="L8" s="5">
         <f t="shared" si="6"/>
-        <v>2908.7999999999997</v>
-      </c>
-      <c r="K8" s="5">
-        <f t="shared" si="7"/>
-        <v>698111.99999999988</v>
-      </c>
-      <c r="L8" s="5">
-        <f t="shared" si="8"/>
-        <v>187.03703703703701</v>
+        <v>22.251157407407408</v>
       </c>
       <c r="M8" s="6" t="b">
         <f t="shared" ref="M8:M16" si="11">IF((F8-FLOOR(F8,1))=0,IF((G8-FLOOR(G8,1))=0,IF((H8-FLOOR(H8,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1235,112 +1235,112 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
+        <v>24</v>
+      </c>
+      <c r="B9" s="4">
+        <v>16</v>
+      </c>
+      <c r="C9" s="4">
         <v>8</v>
-      </c>
-      <c r="B9" s="4">
-        <v>5</v>
-      </c>
-      <c r="C9" s="4">
-        <v>4</v>
       </c>
       <c r="D9" s="5">
         <f t="shared" si="0"/>
-        <v>6.666666666666667</v>
+        <v>128</v>
       </c>
       <c r="E9" s="5">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>3072</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="3"/>
-        <v>16.399999999999999</v>
+        <v>14</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="I9" s="5">
+        <f t="shared" si="7"/>
+        <v>18200</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="8"/>
+        <v>4376</v>
+      </c>
+      <c r="K9" s="5">
         <f t="shared" si="5"/>
-        <v>3607.9999999999995</v>
-      </c>
-      <c r="J9" s="5">
+        <v>13443072</v>
+      </c>
+      <c r="L9" s="5">
         <f t="shared" si="6"/>
-        <v>2913.6</v>
-      </c>
-      <c r="K9" s="5">
-        <f t="shared" si="7"/>
-        <v>466176</v>
-      </c>
-      <c r="L9" s="5">
-        <f t="shared" si="8"/>
-        <v>124.89711934156378</v>
+        <v>31.655092592592592</v>
       </c>
       <c r="M9" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N9" s="6" t="b">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B10" s="4">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C10" s="4">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D10" s="5">
         <f t="shared" si="0"/>
-        <v>6.666666666666667</v>
+        <v>256</v>
       </c>
       <c r="E10" s="5">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>6144</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" si="2"/>
-        <v>9.1999999999999993</v>
+        <v>50</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="I10" s="5">
-        <f t="shared" si="5"/>
-        <v>3680</v>
+        <f t="shared" si="7"/>
+        <v>9800</v>
       </c>
       <c r="J10" s="5">
+        <f t="shared" si="8"/>
+        <v>2888</v>
+      </c>
+      <c r="K10" s="5">
+        <f>J10*E10</f>
+        <v>17743872</v>
+      </c>
+      <c r="L10" s="5">
         <f t="shared" si="6"/>
-        <v>3072</v>
-      </c>
-      <c r="K10" s="5">
-        <f t="shared" si="7"/>
-        <v>491520</v>
-      </c>
-      <c r="L10" s="5">
-        <f t="shared" si="8"/>
-        <v>131.68724279835391</v>
+        <v>41.782407407407405</v>
       </c>
       <c r="M10" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N10" s="6" t="b">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1363,31 +1363,31 @@
       </c>
       <c r="F11" s="5">
         <f t="shared" si="2"/>
-        <v>6.5</v>
+        <v>74</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="3"/>
-        <v>16.399999999999999</v>
+        <v>40.4</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="I11" s="5">
+        <f t="shared" si="7"/>
+        <v>292980.8</v>
+      </c>
+      <c r="J11" s="5">
+        <f t="shared" si="8"/>
+        <v>27560</v>
+      </c>
+      <c r="K11" s="5">
         <f t="shared" si="5"/>
-        <v>4050.7999999999997</v>
-      </c>
-      <c r="J11" s="5">
+        <v>4409600</v>
+      </c>
+      <c r="L11" s="5">
         <f t="shared" si="6"/>
-        <v>3907.2</v>
-      </c>
-      <c r="K11" s="5">
-        <f t="shared" si="7"/>
-        <v>625152</v>
-      </c>
-      <c r="L11" s="5">
-        <f t="shared" si="8"/>
-        <v>167.48971193415639</v>
+        <v>10.383511766975309</v>
       </c>
       <c r="M11" s="6" t="b">
         <f t="shared" si="11"/>
@@ -1418,31 +1418,31 @@
       </c>
       <c r="F12" s="5">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>146</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="I12" s="5">
+        <f t="shared" si="7"/>
+        <v>129064</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" si="8"/>
+        <v>18472</v>
+      </c>
+      <c r="K12" s="5">
         <f t="shared" si="5"/>
-        <v>1694</v>
-      </c>
-      <c r="J12" s="5">
+        <v>7093248</v>
+      </c>
+      <c r="L12" s="5">
         <f t="shared" si="6"/>
-        <v>1716</v>
-      </c>
-      <c r="K12" s="5">
-        <f t="shared" si="7"/>
-        <v>658944</v>
-      </c>
-      <c r="L12" s="5">
-        <f t="shared" si="8"/>
-        <v>176.54320987654322</v>
+        <v>16.702835648148149</v>
       </c>
       <c r="M12" s="6" t="b">
         <f t="shared" si="11"/>
@@ -1473,35 +1473,35 @@
       </c>
       <c r="F13" s="5">
         <f t="shared" si="2"/>
-        <v>6.5</v>
+        <v>74</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="I13" s="5">
+        <f t="shared" si="7"/>
+        <v>185000</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" si="8"/>
+        <v>19112</v>
+      </c>
+      <c r="K13" s="5">
         <f t="shared" si="5"/>
-        <v>2600</v>
-      </c>
-      <c r="J13" s="5">
+        <v>4892672</v>
+      </c>
+      <c r="L13" s="5">
         <f t="shared" si="6"/>
-        <v>2640</v>
-      </c>
-      <c r="K13" s="5">
-        <f t="shared" si="7"/>
-        <v>675840</v>
-      </c>
-      <c r="L13" s="5">
-        <f t="shared" si="8"/>
-        <v>181.06995884773661</v>
+        <v>11.5210262345679</v>
       </c>
       <c r="M13" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" s="6" t="b">
         <f t="shared" si="9"/>
@@ -1528,31 +1528,31 @@
       </c>
       <c r="F14" s="5">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>146</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="H14" s="5">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="I14" s="5">
+        <f t="shared" si="7"/>
+        <v>189800</v>
+      </c>
+      <c r="J14" s="5">
+        <f t="shared" si="8"/>
+        <v>23912</v>
+      </c>
+      <c r="K14" s="5">
         <f t="shared" si="5"/>
-        <v>2420</v>
-      </c>
-      <c r="J14" s="5">
+        <v>6121472</v>
+      </c>
+      <c r="L14" s="5">
         <f t="shared" si="6"/>
-        <v>2244</v>
-      </c>
-      <c r="K14" s="5">
-        <f t="shared" si="7"/>
-        <v>574464</v>
-      </c>
-      <c r="L14" s="5">
-        <f t="shared" si="8"/>
-        <v>153.90946502057614</v>
+        <v>14.414544753086419</v>
       </c>
       <c r="M14" s="6" t="b">
         <f t="shared" si="11"/>
@@ -1583,31 +1583,31 @@
       </c>
       <c r="F15" s="5">
         <f t="shared" si="2"/>
-        <v>6.5</v>
+        <v>74</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="3"/>
-        <v>9.1999999999999993</v>
+        <v>21.2</v>
       </c>
       <c r="H15" s="5">
         <f t="shared" si="4"/>
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="I15" s="5">
+        <f t="shared" si="7"/>
+        <v>153742.39999999999</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" si="8"/>
+        <v>21032</v>
+      </c>
+      <c r="K15" s="5">
         <f t="shared" si="5"/>
-        <v>2272.4</v>
-      </c>
-      <c r="J15" s="5">
+        <v>6730240</v>
+      </c>
+      <c r="L15" s="5">
         <f t="shared" si="6"/>
-        <v>2625.6</v>
-      </c>
-      <c r="K15" s="5">
-        <f t="shared" si="7"/>
-        <v>840192</v>
-      </c>
-      <c r="L15" s="5">
-        <f t="shared" si="8"/>
-        <v>225.10288065843622</v>
+        <v>15.848042052469136</v>
       </c>
       <c r="M15" s="6" t="b">
         <f t="shared" si="11"/>
@@ -1638,31 +1638,31 @@
       </c>
       <c r="F16" s="5">
         <f t="shared" si="2"/>
-        <v>9.1999999999999993</v>
+        <v>117.2</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="I16" s="5">
+        <f t="shared" si="7"/>
+        <v>152360</v>
+      </c>
+      <c r="J16" s="5">
+        <f t="shared" si="8"/>
+        <v>19649.600000000002</v>
+      </c>
+      <c r="K16" s="5">
         <f t="shared" si="5"/>
-        <v>2023.9999999999998</v>
-      </c>
-      <c r="J16" s="5">
+        <v>6287872.0000000009</v>
+      </c>
+      <c r="L16" s="5">
         <f t="shared" si="6"/>
-        <v>2020.8</v>
-      </c>
-      <c r="K16" s="5">
-        <f t="shared" si="7"/>
-        <v>646656</v>
-      </c>
-      <c r="L16" s="5">
-        <f t="shared" si="8"/>
-        <v>173.25102880658437</v>
+        <v>14.806375385802472</v>
       </c>
       <c r="M16" s="6" t="b">
         <f t="shared" si="11"/>
@@ -1689,7 +1689,7 @@
         <v>68</v>
       </c>
       <c r="B20" s="14">
-        <v>1.5</v>
+        <v>192</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>18</v>
@@ -1738,11 +1738,11 @@
         <v>4</v>
       </c>
       <c r="B23" s="15">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="C23" s="3">
         <f>CEILING($B$20*B23,1)</f>
-        <v>72</v>
+        <v>1152</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="17"/>
@@ -1760,11 +1760,11 @@
         <v>5</v>
       </c>
       <c r="B24" s="15">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="C24" s="3">
         <f t="shared" ref="C24:C25" si="12">CEILING($B$20*B24,1)</f>
-        <v>72</v>
+        <v>192</v>
       </c>
       <c r="E24" s="12"/>
       <c r="F24" s="17"/>
@@ -1782,11 +1782,11 @@
         <v>6</v>
       </c>
       <c r="B25" s="15">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="C25" s="3">
         <f t="shared" si="12"/>
-        <v>72</v>
+        <v>192</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
@@ -1804,7 +1804,7 @@
       </c>
       <c r="C26" s="3">
         <f>C23*C24*C25</f>
-        <v>373248</v>
+        <v>42467328</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="17"/>
@@ -2202,8 +2202,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2302,16 +2302,16 @@
         <v>4608</v>
       </c>
       <c r="J2" s="5">
-        <f t="shared" ref="J2:J16" si="6">4*F2*G2+4*G2*H2+4*F2*H2</f>
-        <v>3648</v>
+        <f>((F2*G2) + (G2*(H2-2)) + ((F2-2)*(H2-2)))*2</f>
+        <v>1608</v>
       </c>
       <c r="K2" s="5">
-        <f t="shared" ref="K2:K16" si="7">J2*E2</f>
-        <v>233472</v>
+        <f t="shared" ref="K2:K16" si="6">J2*E2</f>
+        <v>102912</v>
       </c>
       <c r="L2" s="5">
-        <f t="shared" ref="L2:L16" si="8">K2/$C$27*100</f>
-        <v>121.6</v>
+        <f t="shared" ref="L2:L16" si="7">K2/$C$27*100</f>
+        <v>53.6</v>
       </c>
       <c r="M2" s="6" t="b">
         <f>IF((F2-FLOOR(F2,1))=0,IF((G2-FLOOR(G2,1))=0,IF((H2-FLOOR(H2,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -2357,16 +2357,16 @@
         <v>2448</v>
       </c>
       <c r="J3" s="5">
+        <f t="shared" ref="J3:J16" si="8">((F3*G3) + (G3*(H3-2)) + ((F3-2)*(H3-2)))*2</f>
+        <v>948</v>
+      </c>
+      <c r="K3" s="5">
         <f t="shared" si="6"/>
-        <v>2208</v>
-      </c>
-      <c r="K3" s="5">
+        <v>121344</v>
+      </c>
+      <c r="L3" s="5">
         <f t="shared" si="7"/>
-        <v>282624</v>
-      </c>
-      <c r="L3" s="5">
-        <f t="shared" si="8"/>
-        <v>147.19999999999999</v>
+        <v>63.2</v>
       </c>
       <c r="M3" s="6" t="b">
         <f>IF((F3-FLOOR(F3,1))=0,IF((G3-FLOOR(G3,1))=0,IF((H3-FLOOR(H3,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -2412,16 +2412,16 @@
         <v>1768.0000000000002</v>
       </c>
       <c r="J4" s="5">
+        <f t="shared" si="8"/>
+        <v>768</v>
+      </c>
+      <c r="K4" s="5">
         <f t="shared" si="6"/>
-        <v>1821.3333333333335</v>
-      </c>
-      <c r="K4" s="5">
+        <v>147456</v>
+      </c>
+      <c r="L4" s="5">
         <f t="shared" si="7"/>
-        <v>349696</v>
-      </c>
-      <c r="L4" s="5">
-        <f t="shared" si="8"/>
-        <v>182.13333333333333</v>
+        <v>76.8</v>
       </c>
       <c r="M4" s="6" t="b">
         <f t="shared" ref="M4:M6" si="10">IF((F4-FLOOR(F4,1))=0,IF((G4-FLOOR(G4,1))=0,IF((H4-FLOOR(H4,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -2467,16 +2467,16 @@
         <v>1728</v>
       </c>
       <c r="J5" s="5">
+        <f t="shared" si="8"/>
+        <v>728</v>
+      </c>
+      <c r="K5" s="5">
         <f t="shared" si="6"/>
-        <v>1728</v>
-      </c>
-      <c r="K5" s="5">
+        <v>139776</v>
+      </c>
+      <c r="L5" s="5">
         <f t="shared" si="7"/>
-        <v>331776</v>
-      </c>
-      <c r="L5" s="5">
-        <f t="shared" si="8"/>
-        <v>172.8</v>
+        <v>72.8</v>
       </c>
       <c r="M5" s="6" t="b">
         <f t="shared" si="10"/>
@@ -2522,16 +2522,16 @@
         <v>1224</v>
       </c>
       <c r="J6" s="5">
+        <f t="shared" si="8"/>
+        <v>624</v>
+      </c>
+      <c r="K6" s="5">
         <f t="shared" si="6"/>
-        <v>1512</v>
-      </c>
-      <c r="K6" s="5">
+        <v>199680</v>
+      </c>
+      <c r="L6" s="5">
         <f t="shared" si="7"/>
-        <v>483840</v>
-      </c>
-      <c r="L6" s="5">
-        <f t="shared" si="8"/>
-        <v>252</v>
+        <v>104</v>
       </c>
       <c r="M6" s="6" t="b">
         <f t="shared" si="10"/>
@@ -2577,16 +2577,16 @@
         <v>2410.2222222222222</v>
       </c>
       <c r="J7" s="5">
+        <f t="shared" si="8"/>
+        <v>1076.8888888888889</v>
+      </c>
+      <c r="K7" s="5">
         <f t="shared" si="6"/>
-        <v>2501.333333333333</v>
-      </c>
-      <c r="K7" s="5">
+        <v>155072</v>
+      </c>
+      <c r="L7" s="5">
         <f t="shared" si="7"/>
-        <v>360191.99999999994</v>
-      </c>
-      <c r="L7" s="5">
-        <f t="shared" si="8"/>
-        <v>187.59999999999997</v>
+        <v>80.766666666666666</v>
       </c>
       <c r="M7" s="6" t="b">
         <f>IF((F7-FLOOR(F7,1))=0,IF((G7-FLOOR(G7,1))=0,IF((H7-FLOOR(H7,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -2632,16 +2632,16 @@
         <v>5208</v>
       </c>
       <c r="J8" s="5">
+        <f t="shared" si="8"/>
+        <v>2208</v>
+      </c>
+      <c r="K8" s="5">
         <f t="shared" si="6"/>
-        <v>5048</v>
-      </c>
-      <c r="K8" s="5">
+        <v>141312</v>
+      </c>
+      <c r="L8" s="5">
         <f t="shared" si="7"/>
-        <v>323072</v>
-      </c>
-      <c r="L8" s="5">
-        <f t="shared" si="8"/>
-        <v>168.26666666666668</v>
+        <v>73.599999999999994</v>
       </c>
       <c r="M8" s="6" t="b">
         <f t="shared" ref="M8:M16" si="11">IF((F8-FLOOR(F8,1))=0,IF((G8-FLOOR(G8,1))=0,IF((H8-FLOOR(H8,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -2687,16 +2687,16 @@
         <v>3038</v>
       </c>
       <c r="J9" s="5">
+        <f t="shared" si="8"/>
+        <v>1538</v>
+      </c>
+      <c r="K9" s="5">
         <f t="shared" si="6"/>
-        <v>3668</v>
-      </c>
-      <c r="K9" s="5">
+        <v>196864</v>
+      </c>
+      <c r="L9" s="5">
         <f t="shared" si="7"/>
-        <v>469504</v>
-      </c>
-      <c r="L9" s="5">
-        <f t="shared" si="8"/>
-        <v>244.5333333333333</v>
+        <v>102.53333333333335</v>
       </c>
       <c r="M9" s="6" t="b">
         <f t="shared" si="11"/>
@@ -2742,16 +2742,16 @@
         <v>2314.666666666667</v>
       </c>
       <c r="J10" s="5">
+        <f t="shared" si="8"/>
+        <v>1314.6666666666667</v>
+      </c>
+      <c r="K10" s="5">
         <f t="shared" si="6"/>
-        <v>3208</v>
-      </c>
-      <c r="K10" s="5">
+        <v>252416</v>
+      </c>
+      <c r="L10" s="5">
         <f t="shared" si="7"/>
-        <v>615936</v>
-      </c>
-      <c r="L10" s="5">
-        <f t="shared" si="8"/>
-        <v>320.8</v>
+        <v>131.46666666666667</v>
       </c>
       <c r="M10" s="6" t="b">
         <f t="shared" si="11"/>
@@ -2797,16 +2797,16 @@
         <v>1953</v>
       </c>
       <c r="J11" s="5">
+        <f t="shared" si="8"/>
+        <v>1203</v>
+      </c>
+      <c r="K11" s="5">
         <f t="shared" si="6"/>
-        <v>2978</v>
-      </c>
-      <c r="K11" s="5">
+        <v>307968</v>
+      </c>
+      <c r="L11" s="5">
         <f t="shared" si="7"/>
-        <v>762368</v>
-      </c>
-      <c r="L11" s="5">
-        <f t="shared" si="8"/>
-        <v>397.06666666666666</v>
+        <v>160.4</v>
       </c>
       <c r="M11" s="6" t="b">
         <f t="shared" si="11"/>
@@ -2852,16 +2852,16 @@
         <v>1736</v>
       </c>
       <c r="J12" s="5">
+        <f t="shared" si="8"/>
+        <v>1136</v>
+      </c>
+      <c r="K12" s="5">
         <f t="shared" si="6"/>
-        <v>2840</v>
-      </c>
-      <c r="K12" s="5">
+        <v>363520</v>
+      </c>
+      <c r="L12" s="5">
         <f t="shared" si="7"/>
-        <v>908800</v>
-      </c>
-      <c r="L12" s="5">
-        <f t="shared" si="8"/>
-        <v>473.33333333333331</v>
+        <v>189.33333333333334</v>
       </c>
       <c r="M12" s="6" t="b">
         <f t="shared" si="11"/>
@@ -2907,16 +2907,16 @@
         <v>766.88888888888891</v>
       </c>
       <c r="J13" s="5">
+        <f t="shared" si="8"/>
+        <v>433.55555555555554</v>
+      </c>
+      <c r="K13" s="5">
         <f t="shared" si="6"/>
-        <v>1094.6666666666667</v>
-      </c>
-      <c r="K13" s="5">
+        <v>249728</v>
+      </c>
+      <c r="L13" s="5">
         <f t="shared" si="7"/>
-        <v>630528</v>
-      </c>
-      <c r="L13" s="5">
-        <f t="shared" si="8"/>
-        <v>328.4</v>
+        <v>130.06666666666666</v>
       </c>
       <c r="M13" s="6" t="b">
         <f t="shared" si="11"/>
@@ -2962,16 +2962,16 @@
         <v>15488</v>
       </c>
       <c r="J14" s="5">
+        <f t="shared" si="8"/>
+        <v>3488</v>
+      </c>
+      <c r="K14" s="5">
         <f t="shared" si="6"/>
-        <v>7568</v>
-      </c>
-      <c r="K14" s="5">
+        <v>55808</v>
+      </c>
+      <c r="L14" s="5">
         <f t="shared" si="7"/>
-        <v>121088</v>
-      </c>
-      <c r="L14" s="5">
-        <f t="shared" si="8"/>
-        <v>63.06666666666667</v>
+        <v>29.06666666666667</v>
       </c>
       <c r="M14" s="6" t="b">
         <f t="shared" si="11"/>
@@ -3017,16 +3017,16 @@
         <v>29568</v>
       </c>
       <c r="J15" s="5">
+        <f t="shared" si="8"/>
+        <v>5568</v>
+      </c>
+      <c r="K15" s="5">
         <f t="shared" si="6"/>
-        <v>11888</v>
-      </c>
-      <c r="K15" s="5">
+        <v>44544</v>
+      </c>
+      <c r="L15" s="5">
         <f t="shared" si="7"/>
-        <v>95104</v>
-      </c>
-      <c r="L15" s="5">
-        <f t="shared" si="8"/>
-        <v>49.533333333333331</v>
+        <v>23.200000000000003</v>
       </c>
       <c r="M15" s="6" t="b">
         <f t="shared" si="11"/>
@@ -3072,16 +3072,16 @@
         <v>665</v>
       </c>
       <c r="J16" s="5">
+        <f t="shared" si="8"/>
+        <v>365</v>
+      </c>
+      <c r="K16" s="5">
         <f t="shared" si="6"/>
-        <v>926</v>
-      </c>
-      <c r="K16" s="5">
+        <v>233600</v>
+      </c>
+      <c r="L16" s="5">
         <f t="shared" si="7"/>
-        <v>592640</v>
-      </c>
-      <c r="L16" s="5">
-        <f t="shared" si="8"/>
-        <v>308.66666666666663</v>
+        <v>121.66666666666666</v>
       </c>
       <c r="M16" s="6" t="b">
         <f t="shared" si="11"/>
@@ -3571,8 +3571,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3671,16 +3671,16 @@
         <v>2750280</v>
       </c>
       <c r="J2" s="5">
-        <f t="shared" ref="J2:J16" si="6">4*F2*G2+4*G2*H2+4*F2*H2</f>
-        <v>261424</v>
+        <f>((F2*G2) + (G2*(H2-2)) + ((F2-2)*(H2-2)))*2</f>
+        <v>128840</v>
       </c>
       <c r="K2" s="5">
-        <f t="shared" ref="K2:K16" si="7">J2*E2</f>
-        <v>3137088</v>
+        <f t="shared" ref="K2:K16" si="6">J2*E2</f>
+        <v>1546080</v>
       </c>
       <c r="L2" s="5">
-        <f t="shared" ref="L2:L16" si="8">K2/$C$27*100</f>
-        <v>9.9725341796875</v>
+        <f t="shared" ref="L2:L16" si="7">K2/$C$27*100</f>
+        <v>4.91485595703125</v>
       </c>
       <c r="M2" s="6" t="b">
         <f>IF((F2-FLOOR(F2,1))=0,IF((G2-FLOOR(G2,1))=0,IF((H2-FLOOR(H2,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -3726,16 +3726,16 @@
         <v>1385800</v>
       </c>
       <c r="J3" s="5">
+        <f t="shared" ref="J3:J16" si="8">((F3*G3) + (G3*(H3-2)) + ((F3-2)*(H3-2)))*2</f>
+        <v>75080</v>
+      </c>
+      <c r="K3" s="5">
         <f t="shared" si="6"/>
-        <v>152880</v>
-      </c>
-      <c r="K3" s="5">
+        <v>1801920</v>
+      </c>
+      <c r="L3" s="5">
         <f t="shared" si="7"/>
-        <v>3669120</v>
-      </c>
-      <c r="L3" s="5">
-        <f t="shared" si="8"/>
-        <v>11.663818359375</v>
+        <v>5.7281494140625</v>
       </c>
       <c r="M3" s="6" t="b">
         <f>IF((F3-FLOOR(F3,1))=0,IF((G3-FLOOR(G3,1))=0,IF((H3-FLOOR(H3,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -3781,16 +3781,16 @@
         <v>935133.33333333337</v>
       </c>
       <c r="J4" s="5">
+        <f t="shared" si="8"/>
+        <v>61320</v>
+      </c>
+      <c r="K4" s="5">
         <f t="shared" si="6"/>
-        <v>125146.66666666667</v>
-      </c>
-      <c r="K4" s="5">
+        <v>2207520</v>
+      </c>
+      <c r="L4" s="5">
         <f t="shared" si="7"/>
-        <v>4505280</v>
-      </c>
-      <c r="L4" s="5">
-        <f t="shared" si="8"/>
-        <v>14.3218994140625</v>
+        <v>7.01751708984375</v>
       </c>
       <c r="M4" s="6" t="b">
         <f t="shared" ref="M4:M6" si="10">IF((F4-FLOOR(F4,1))=0,IF((G4-FLOOR(G4,1))=0,IF((H4-FLOOR(H4,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -3836,16 +3836,16 @@
         <v>325462.22222222225</v>
       </c>
       <c r="J5" s="5">
+        <f t="shared" si="8"/>
+        <v>34191.111111111109</v>
+      </c>
+      <c r="K5" s="5">
         <f t="shared" si="6"/>
-        <v>70334.222222222219</v>
-      </c>
-      <c r="K5" s="5">
+        <v>3692640</v>
+      </c>
+      <c r="L5" s="5">
         <f t="shared" si="7"/>
-        <v>7596096</v>
-      </c>
-      <c r="L5" s="5">
-        <f t="shared" si="8"/>
-        <v>24.1473388671875</v>
+        <v>11.73858642578125</v>
       </c>
       <c r="M5" s="6" t="b">
         <f t="shared" si="10"/>
@@ -3891,16 +3891,16 @@
         <v>1059240</v>
       </c>
       <c r="J6" s="5">
+        <f t="shared" si="8"/>
+        <v>76200</v>
+      </c>
+      <c r="K6" s="5">
         <f t="shared" si="6"/>
-        <v>155312</v>
-      </c>
-      <c r="K6" s="5">
+        <v>2438400</v>
+      </c>
+      <c r="L6" s="5">
         <f t="shared" si="7"/>
-        <v>4969984</v>
-      </c>
-      <c r="L6" s="5">
-        <f t="shared" si="8"/>
-        <v>15.799153645833334</v>
+        <v>7.75146484375</v>
       </c>
       <c r="M6" s="6" t="b">
         <f t="shared" si="10"/>
@@ -3946,16 +3946,16 @@
         <v>368424</v>
       </c>
       <c r="J7" s="5">
+        <f t="shared" si="8"/>
+        <v>40744</v>
+      </c>
+      <c r="K7" s="5">
         <f t="shared" si="6"/>
-        <v>84144</v>
-      </c>
-      <c r="K7" s="5">
+        <v>3911424</v>
+      </c>
+      <c r="L7" s="5">
         <f t="shared" si="7"/>
-        <v>8077824</v>
-      </c>
-      <c r="L7" s="5">
-        <f t="shared" si="8"/>
-        <v>25.6787109375</v>
+        <v>12.43408203125</v>
       </c>
       <c r="M7" s="6" t="b">
         <f>IF((F7-FLOOR(F7,1))=0,IF((G7-FLOOR(G7,1))=0,IF((H7-FLOOR(H7,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -4001,16 +4001,16 @@
         <v>192984</v>
       </c>
       <c r="J8" s="5">
+        <f t="shared" si="8"/>
+        <v>29144</v>
+      </c>
+      <c r="K8" s="5">
         <f t="shared" si="6"/>
-        <v>60784</v>
-      </c>
-      <c r="K8" s="5">
+        <v>5595648</v>
+      </c>
+      <c r="L8" s="5">
         <f t="shared" si="7"/>
-        <v>11670528</v>
-      </c>
-      <c r="L8" s="5">
-        <f t="shared" si="8"/>
-        <v>37.099609375</v>
+        <v>17.7880859375</v>
       </c>
       <c r="M8" s="6" t="b">
         <f t="shared" ref="M8:M16" si="11">IF((F8-FLOOR(F8,1))=0,IF((G8-FLOOR(G8,1))=0,IF((H8-FLOOR(H8,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -4056,16 +4056,16 @@
         <v>97240</v>
       </c>
       <c r="J9" s="5">
+        <f t="shared" si="8"/>
+        <v>15320</v>
+      </c>
+      <c r="K9" s="5">
         <f t="shared" si="6"/>
-        <v>32112</v>
-      </c>
-      <c r="K9" s="5">
+        <v>5882880</v>
+      </c>
+      <c r="L9" s="5">
         <f t="shared" si="7"/>
-        <v>12331008</v>
-      </c>
-      <c r="L9" s="5">
-        <f t="shared" si="8"/>
-        <v>39.19921875</v>
+        <v>18.701171875</v>
       </c>
       <c r="M9" s="6" t="b">
         <f t="shared" si="11"/>
@@ -4111,16 +4111,16 @@
         <v>218433.6</v>
       </c>
       <c r="J10" s="5">
+        <f t="shared" si="8"/>
+        <v>21825.599999999999</v>
+      </c>
+      <c r="K10" s="5">
         <f t="shared" si="6"/>
-        <v>45129.600000000006</v>
-      </c>
-      <c r="K10" s="5">
+        <v>3492096</v>
+      </c>
+      <c r="L10" s="5">
         <f t="shared" si="7"/>
-        <v>7220736.0000000009</v>
-      </c>
-      <c r="L10" s="5">
-        <f t="shared" si="8"/>
-        <v>22.954101562500004</v>
+        <v>11.10107421875</v>
       </c>
       <c r="M10" s="6" t="b">
         <f t="shared" si="11"/>
@@ -4166,16 +4166,16 @@
         <v>221000</v>
       </c>
       <c r="J11" s="5">
+        <f t="shared" si="8"/>
+        <v>24392</v>
+      </c>
+      <c r="K11" s="5">
         <f t="shared" si="6"/>
-        <v>50480</v>
-      </c>
-      <c r="K11" s="5">
+        <v>3902720</v>
+      </c>
+      <c r="L11" s="5">
         <f t="shared" si="7"/>
-        <v>8076800</v>
-      </c>
-      <c r="L11" s="5">
-        <f t="shared" si="8"/>
-        <v>25.675455729166668</v>
+        <v>12.406412760416668</v>
       </c>
       <c r="M11" s="6" t="b">
         <f t="shared" si="11"/>
@@ -4221,16 +4221,16 @@
         <v>188290.66666666666</v>
       </c>
       <c r="J12" s="5">
+        <f t="shared" si="8"/>
+        <v>24450.666666666664</v>
+      </c>
+      <c r="K12" s="5">
         <f t="shared" si="6"/>
-        <v>50544</v>
-      </c>
-      <c r="K12" s="5">
+        <v>4694528</v>
+      </c>
+      <c r="L12" s="5">
         <f t="shared" si="7"/>
-        <v>9704448</v>
-      </c>
-      <c r="L12" s="5">
-        <f t="shared" si="8"/>
-        <v>30.849609374999996</v>
+        <v>14.923502604166666</v>
       </c>
       <c r="M12" s="6" t="b">
         <f t="shared" si="11"/>
@@ -4276,16 +4276,16 @@
         <v>138600</v>
       </c>
       <c r="J13" s="5">
+        <f t="shared" si="8"/>
+        <v>15720</v>
+      </c>
+      <c r="K13" s="5">
         <f t="shared" si="6"/>
-        <v>32688</v>
-      </c>
-      <c r="K13" s="5">
+        <v>4024320</v>
+      </c>
+      <c r="L13" s="5">
         <f t="shared" si="7"/>
-        <v>8368128</v>
-      </c>
-      <c r="L13" s="5">
-        <f t="shared" si="8"/>
-        <v>26.601562499999996</v>
+        <v>12.79296875</v>
       </c>
       <c r="M13" s="6" t="b">
         <f t="shared" si="11"/>
@@ -4331,16 +4331,16 @@
         <v>142296</v>
       </c>
       <c r="J14" s="5">
+        <f t="shared" si="8"/>
+        <v>19416</v>
+      </c>
+      <c r="K14" s="5">
         <f t="shared" si="6"/>
-        <v>40304</v>
-      </c>
-      <c r="K14" s="5">
+        <v>4970496</v>
+      </c>
+      <c r="L14" s="5">
         <f t="shared" si="7"/>
-        <v>10317824</v>
-      </c>
-      <c r="L14" s="5">
-        <f t="shared" si="8"/>
-        <v>32.799479166666664</v>
+        <v>15.800781250000002</v>
       </c>
       <c r="M14" s="6" t="b">
         <f t="shared" si="11"/>
@@ -4386,16 +4386,16 @@
         <v>117000</v>
       </c>
       <c r="J15" s="5">
+        <f t="shared" si="8"/>
+        <v>18696</v>
+      </c>
+      <c r="K15" s="5">
         <f t="shared" si="6"/>
-        <v>38960</v>
-      </c>
-      <c r="K15" s="5">
+        <v>5982720</v>
+      </c>
+      <c r="L15" s="5">
         <f t="shared" si="7"/>
-        <v>12467200</v>
-      </c>
-      <c r="L15" s="5">
-        <f t="shared" si="8"/>
-        <v>39.632161458333329</v>
+        <v>19.0185546875</v>
       </c>
       <c r="M15" s="6" t="b">
         <f t="shared" si="11"/>
@@ -4441,16 +4441,16 @@
         <v>97240</v>
       </c>
       <c r="J16" s="5">
+        <f t="shared" si="8"/>
+        <v>15320</v>
+      </c>
+      <c r="K16" s="5">
         <f t="shared" si="6"/>
-        <v>32112</v>
-      </c>
-      <c r="K16" s="5">
+        <v>5882880</v>
+      </c>
+      <c r="L16" s="5">
         <f t="shared" si="7"/>
-        <v>12331008</v>
-      </c>
-      <c r="L16" s="5">
-        <f t="shared" si="8"/>
-        <v>39.19921875</v>
+        <v>18.701171875</v>
       </c>
       <c r="M16" s="6" t="b">
         <f t="shared" si="11"/>
@@ -4594,8 +4594,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24:J36"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4694,16 +4694,16 @@
         <v>2068040</v>
       </c>
       <c r="J2" s="5">
-        <f t="shared" ref="J2:J16" si="6">4*F2*G2+4*G2*H2+4*F2*H2</f>
-        <v>207152</v>
+        <f>((F2*G2) + (G2*(H2-2)) + ((F2-2)*(H2-2)))*2</f>
+        <v>101960</v>
       </c>
       <c r="K2" s="5">
-        <f t="shared" ref="K2:K16" si="7">J2*E2</f>
-        <v>3314432</v>
+        <f t="shared" ref="K2:K16" si="6">J2*E2</f>
+        <v>1631360</v>
       </c>
       <c r="L2" s="5">
-        <f t="shared" ref="L2:L16" si="8">K2/$C$27*100</f>
-        <v>10.536295572916666</v>
+        <f t="shared" ref="L2:L16" si="7">K2/$C$27*100</f>
+        <v>5.1859537760416661</v>
       </c>
       <c r="M2" s="6" t="b">
         <f>IF((F2-FLOOR(F2,1))=0,IF((G2-FLOOR(G2,1))=0,IF((H2-FLOOR(H2,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -4749,16 +4749,16 @@
         <v>1706120</v>
       </c>
       <c r="J3" s="5">
+        <f t="shared" ref="J3:J16" si="8">((F3*G3) + (G3*(H3-2)) + ((F3-2)*(H3-2)))*2</f>
+        <v>133256</v>
+      </c>
+      <c r="K3" s="5">
         <f t="shared" si="6"/>
-        <v>270896</v>
-      </c>
-      <c r="K3" s="5">
+        <v>2665120</v>
+      </c>
+      <c r="L3" s="5">
         <f t="shared" si="7"/>
-        <v>5417920</v>
-      </c>
-      <c r="L3" s="5">
-        <f t="shared" si="8"/>
-        <v>17.223103841145836</v>
+        <v>8.4721883138020821</v>
       </c>
       <c r="M3" s="6" t="b">
         <f>IF((F3-FLOOR(F3,1))=0,IF((G3-FLOOR(G3,1))=0,IF((H3-FLOOR(H3,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -4804,16 +4804,16 @@
         <v>1658695.9999999998</v>
       </c>
       <c r="J4" s="5">
+        <f t="shared" si="8"/>
+        <v>85832</v>
+      </c>
+      <c r="K4" s="5">
         <f t="shared" si="6"/>
-        <v>174588.79999999999</v>
-      </c>
-      <c r="K4" s="5">
+        <v>1716640</v>
+      </c>
+      <c r="L4" s="5">
         <f t="shared" si="7"/>
-        <v>3491776</v>
-      </c>
-      <c r="L4" s="5">
-        <f t="shared" si="8"/>
-        <v>11.100056966145834</v>
+        <v>5.4570515950520839</v>
       </c>
       <c r="M4" s="6" t="b">
         <f t="shared" ref="M4:M6" si="10">IF((F4-FLOOR(F4,1))=0,IF((G4-FLOOR(G4,1))=0,IF((H4-FLOOR(H4,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -4859,16 +4859,16 @@
         <v>4114760</v>
       </c>
       <c r="J5" s="5">
+        <f t="shared" si="8"/>
+        <v>182600</v>
+      </c>
+      <c r="K5" s="5">
         <f t="shared" si="6"/>
-        <v>369968</v>
-      </c>
-      <c r="K5" s="5">
+        <v>1460800</v>
+      </c>
+      <c r="L5" s="5">
         <f t="shared" si="7"/>
-        <v>2959744</v>
-      </c>
-      <c r="L5" s="5">
-        <f t="shared" si="8"/>
-        <v>9.4087727864583339</v>
+        <v>4.6437581380208339</v>
       </c>
       <c r="M5" s="6" t="b">
         <f t="shared" si="10"/>
@@ -4914,16 +4914,16 @@
         <v>1059240</v>
       </c>
       <c r="J6" s="5">
+        <f t="shared" si="8"/>
+        <v>76200</v>
+      </c>
+      <c r="K6" s="5">
         <f t="shared" si="6"/>
-        <v>155312</v>
-      </c>
-      <c r="K6" s="5">
+        <v>2438400</v>
+      </c>
+      <c r="L6" s="5">
         <f t="shared" si="7"/>
-        <v>4969984</v>
-      </c>
-      <c r="L6" s="5">
-        <f t="shared" si="8"/>
-        <v>15.799153645833334</v>
+        <v>7.75146484375</v>
       </c>
       <c r="M6" s="6" t="b">
         <f t="shared" si="10"/>
@@ -4969,16 +4969,16 @@
         <v>537768</v>
       </c>
       <c r="J7" s="5">
+        <f t="shared" si="8"/>
+        <v>46248</v>
+      </c>
+      <c r="K7" s="5">
         <f t="shared" si="6"/>
-        <v>94896</v>
-      </c>
-      <c r="K7" s="5">
+        <v>2959872</v>
+      </c>
+      <c r="L7" s="5">
         <f t="shared" si="7"/>
-        <v>6073344</v>
-      </c>
-      <c r="L7" s="5">
-        <f t="shared" si="8"/>
-        <v>19.306640625</v>
+        <v>9.4091796875</v>
       </c>
       <c r="M7" s="6" t="b">
         <f>IF((F7-FLOOR(F7,1))=0,IF((G7-FLOOR(G7,1))=0,IF((H7-FLOOR(H7,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -5024,16 +5024,16 @@
         <v>271656</v>
       </c>
       <c r="J8" s="5">
+        <f t="shared" si="8"/>
+        <v>25896</v>
+      </c>
+      <c r="K8" s="5">
         <f t="shared" si="6"/>
-        <v>53424</v>
-      </c>
-      <c r="K8" s="5">
+        <v>3314688</v>
+      </c>
+      <c r="L8" s="5">
         <f t="shared" si="7"/>
-        <v>6838272</v>
-      </c>
-      <c r="L8" s="5">
-        <f t="shared" si="8"/>
-        <v>21.73828125</v>
+        <v>10.537109375</v>
       </c>
       <c r="M8" s="6" t="b">
         <f t="shared" ref="M8:M16" si="11">IF((F8-FLOOR(F8,1))=0,IF((G8-FLOOR(G8,1))=0,IF((H8-FLOOR(H8,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -5079,16 +5079,16 @@
         <v>219912</v>
       </c>
       <c r="J9" s="5">
+        <f t="shared" si="8"/>
+        <v>23304</v>
+      </c>
+      <c r="K9" s="5">
         <f t="shared" si="6"/>
-        <v>48176</v>
-      </c>
-      <c r="K9" s="5">
+        <v>3728640</v>
+      </c>
+      <c r="L9" s="5">
         <f t="shared" si="7"/>
-        <v>7708160</v>
-      </c>
-      <c r="L9" s="5">
-        <f t="shared" si="8"/>
-        <v>24.503580729166664</v>
+        <v>11.85302734375</v>
       </c>
       <c r="M9" s="6" t="b">
         <f t="shared" si="11"/>
@@ -5134,16 +5134,16 @@
         <v>218433.6</v>
       </c>
       <c r="J10" s="5">
+        <f t="shared" si="8"/>
+        <v>21825.599999999999</v>
+      </c>
+      <c r="K10" s="5">
         <f t="shared" si="6"/>
-        <v>45129.600000000006</v>
-      </c>
-      <c r="K10" s="5">
+        <v>3492096</v>
+      </c>
+      <c r="L10" s="5">
         <f t="shared" si="7"/>
-        <v>7220736.0000000009</v>
-      </c>
-      <c r="L10" s="5">
-        <f t="shared" si="8"/>
-        <v>22.954101562500004</v>
+        <v>11.10107421875</v>
       </c>
       <c r="M10" s="6" t="b">
         <f t="shared" si="11"/>
@@ -5189,16 +5189,16 @@
         <v>221000</v>
       </c>
       <c r="J11" s="5">
+        <f t="shared" si="8"/>
+        <v>24392</v>
+      </c>
+      <c r="K11" s="5">
         <f t="shared" si="6"/>
-        <v>50480</v>
-      </c>
-      <c r="K11" s="5">
+        <v>3902720</v>
+      </c>
+      <c r="L11" s="5">
         <f t="shared" si="7"/>
-        <v>8076800</v>
-      </c>
-      <c r="L11" s="5">
-        <f t="shared" si="8"/>
-        <v>25.675455729166668</v>
+        <v>12.406412760416668</v>
       </c>
       <c r="M11" s="6" t="b">
         <f t="shared" si="11"/>
@@ -5244,16 +5244,16 @@
         <v>188290.66666666666</v>
       </c>
       <c r="J12" s="5">
+        <f t="shared" si="8"/>
+        <v>24450.666666666664</v>
+      </c>
+      <c r="K12" s="5">
         <f t="shared" si="6"/>
-        <v>50544</v>
-      </c>
-      <c r="K12" s="5">
+        <v>4694528</v>
+      </c>
+      <c r="L12" s="5">
         <f t="shared" si="7"/>
-        <v>9704448</v>
-      </c>
-      <c r="L12" s="5">
-        <f t="shared" si="8"/>
-        <v>30.849609374999996</v>
+        <v>14.923502604166666</v>
       </c>
       <c r="M12" s="6" t="b">
         <f t="shared" si="11"/>
@@ -5299,16 +5299,16 @@
         <v>138600</v>
       </c>
       <c r="J13" s="5">
+        <f t="shared" si="8"/>
+        <v>15720</v>
+      </c>
+      <c r="K13" s="5">
         <f t="shared" si="6"/>
-        <v>32688</v>
-      </c>
-      <c r="K13" s="5">
+        <v>4024320</v>
+      </c>
+      <c r="L13" s="5">
         <f t="shared" si="7"/>
-        <v>8368128</v>
-      </c>
-      <c r="L13" s="5">
-        <f t="shared" si="8"/>
-        <v>26.601562499999996</v>
+        <v>12.79296875</v>
       </c>
       <c r="M13" s="6" t="b">
         <f t="shared" si="11"/>
@@ -5354,16 +5354,16 @@
         <v>182952</v>
       </c>
       <c r="J14" s="5">
+        <f t="shared" si="8"/>
+        <v>19112</v>
+      </c>
+      <c r="K14" s="5">
         <f t="shared" si="6"/>
-        <v>39600</v>
-      </c>
-      <c r="K14" s="5">
+        <v>3669504</v>
+      </c>
+      <c r="L14" s="5">
         <f t="shared" si="7"/>
-        <v>7603200</v>
-      </c>
-      <c r="L14" s="5">
-        <f t="shared" si="8"/>
-        <v>24.169921875</v>
+        <v>11.6650390625</v>
       </c>
       <c r="M14" s="6" t="b">
         <f t="shared" si="11"/>
@@ -5409,16 +5409,16 @@
         <v>113288</v>
       </c>
       <c r="J15" s="5">
+        <f t="shared" si="8"/>
+        <v>14984</v>
+      </c>
+      <c r="K15" s="5">
         <f t="shared" si="6"/>
-        <v>31280</v>
-      </c>
-      <c r="K15" s="5">
+        <v>4794880</v>
+      </c>
+      <c r="L15" s="5">
         <f t="shared" si="7"/>
-        <v>10009600</v>
-      </c>
-      <c r="L15" s="5">
-        <f t="shared" si="8"/>
-        <v>31.819661458333332</v>
+        <v>15.242513020833334</v>
       </c>
       <c r="M15" s="6" t="b">
         <f t="shared" si="11"/>
@@ -5464,16 +5464,16 @@
         <v>58942.399999999994</v>
       </c>
       <c r="J16" s="5">
+        <f t="shared" si="8"/>
+        <v>9790.4</v>
+      </c>
+      <c r="K16" s="5">
         <f t="shared" si="6"/>
-        <v>20643.199999999997</v>
-      </c>
-      <c r="K16" s="5">
+        <v>6265856</v>
+      </c>
+      <c r="L16" s="5">
         <f t="shared" si="7"/>
-        <v>13211647.999999998</v>
-      </c>
-      <c r="L16" s="5">
-        <f t="shared" si="8"/>
-        <v>41.998697916666657</v>
+        <v>19.918619791666668</v>
       </c>
       <c r="M16" s="6" t="b">
         <f t="shared" si="11"/>
@@ -5618,7 +5618,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="J3" sqref="J2:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5716,16 +5716,16 @@
         <v>34383908</v>
       </c>
       <c r="J2" s="5">
-        <f t="shared" ref="J2:J4" si="2">4*F2*G2+4*G2*H2+4*F2*H2</f>
-        <v>1275648</v>
+        <f>((F2*G2) + (G2*(H2-2)) + ((F2-2)*(H2-2)))*2</f>
+        <v>633908</v>
       </c>
       <c r="K2" s="5">
-        <f t="shared" ref="K2:K4" si="3">J2*E2</f>
-        <v>20410368</v>
+        <f t="shared" ref="K2:K4" si="2">J2*E2</f>
+        <v>10142528</v>
       </c>
       <c r="L2" s="5">
         <f>K2/$C$15*100</f>
-        <v>3.7796977777777774</v>
+        <v>1.8782459259259259</v>
       </c>
       <c r="M2" s="6" t="b">
         <f>IF((F2-FLOOR(F2,1))=0,IF((G2-FLOOR(G2,1))=0,IF((H2-FLOOR(H2,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -5771,16 +5771,16 @@
         <v>34519808</v>
       </c>
       <c r="J3" s="5">
+        <f t="shared" ref="J3:J4" si="3">((F3*G3) + (G3*(H3-2)) + ((F3-2)*(H3-2)))*2</f>
+        <v>769808</v>
+      </c>
+      <c r="K3" s="5">
         <f t="shared" si="2"/>
-        <v>1549248</v>
-      </c>
-      <c r="K3" s="5">
-        <f t="shared" si="3"/>
-        <v>24787968</v>
+        <v>12316928</v>
       </c>
       <c r="L3" s="5">
         <f>K3/$C$15*100</f>
-        <v>4.5903644444444449</v>
+        <v>2.2809125925925926</v>
       </c>
       <c r="M3" s="6" t="b">
         <f>IF((F3-FLOOR(F3,1))=0,IF((G3-FLOOR(G3,1))=0,IF((H3-FLOOR(H3,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -5826,16 +5826,16 @@
         <v>34519808</v>
       </c>
       <c r="J4" s="5">
+        <f t="shared" si="3"/>
+        <v>769808</v>
+      </c>
+      <c r="K4" s="5">
         <f t="shared" si="2"/>
-        <v>1549248</v>
-      </c>
-      <c r="K4" s="5">
-        <f t="shared" si="3"/>
-        <v>24787968</v>
+        <v>12316928</v>
       </c>
       <c r="L4" s="5">
         <f>K4/$C$15*100</f>
-        <v>4.5903644444444449</v>
+        <v>2.2809125925925926</v>
       </c>
       <c r="M4" s="6" t="b">
         <f t="shared" ref="M4" si="5">IF((F4-FLOOR(F4,1))=0,IF((G4-FLOOR(G4,1))=0,IF((H4-FLOOR(H4,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -5945,8 +5945,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6044,16 +6044,16 @@
         <v>29568</v>
       </c>
       <c r="J2" s="5">
-        <f t="shared" ref="J2" si="2">4*F2*G2+4*G2*H2+4*F2*H2</f>
-        <v>11888</v>
+        <f>((F2*G2) + (G2*(H2-2)) + ((F2-2)*(H2-2)))*2</f>
+        <v>5568</v>
       </c>
       <c r="K2" s="5">
-        <f t="shared" ref="K2" si="3">J2*E2</f>
-        <v>95104</v>
+        <f t="shared" ref="K2" si="2">J2*E2</f>
+        <v>44544</v>
       </c>
       <c r="L2" s="5">
         <f>K2/$C$14*100</f>
-        <v>49.533333333333331</v>
+        <v>23.200000000000003</v>
       </c>
       <c r="M2" s="6" t="b">
         <f>IF((F2-FLOOR(F2,1))=0,IF((G2-FLOOR(G2,1))=0,IF((H2-FLOOR(H2,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -6079,7 +6079,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" ref="E3" si="4">A3*B3*C3</f>
+        <f t="shared" ref="E3" si="3">A3*B3*C3</f>
         <v>16</v>
       </c>
       <c r="F3" s="5">
@@ -6095,20 +6095,20 @@
         <v>32</v>
       </c>
       <c r="I3" s="5">
-        <f t="shared" ref="I3" si="5">F3*G3*H3</f>
+        <f t="shared" ref="I3" si="4">F3*G3*H3</f>
         <v>15488</v>
       </c>
       <c r="J3" s="5">
-        <f t="shared" ref="J3" si="6">4*F3*G3+4*G3*H3+4*F3*H3</f>
-        <v>7568</v>
+        <f>((F3*G3) + (G3*(H3-2)) + ((F3-2)*(H3-2)))*2</f>
+        <v>3488</v>
       </c>
       <c r="K3" s="5">
-        <f t="shared" ref="K3" si="7">J3*E3</f>
-        <v>121088</v>
+        <f t="shared" ref="K3" si="5">J3*E3</f>
+        <v>55808</v>
       </c>
       <c r="L3" s="5">
         <f>K3/$C$14*100</f>
-        <v>63.06666666666667</v>
+        <v>29.06666666666667</v>
       </c>
       <c r="M3" s="6" t="b">
         <f>IF((F3-FLOOR(F3,1))=0,IF((G3-FLOOR(G3,1))=0,IF((H3-FLOOR(H3,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -6203,7 +6203,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="3">
-        <f t="shared" ref="C12:C13" si="8">$B$7*B12</f>
+        <f t="shared" ref="C12:C13" si="6">$B$7*B12</f>
         <v>40</v>
       </c>
       <c r="E12" s="12"/>
@@ -6225,7 +6225,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
       <c r="J13" s="12"/>
@@ -6576,7 +6576,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:N2">
+  <conditionalFormatting sqref="A2:N2 J3">
     <cfRule type="expression" dxfId="3" priority="3">
       <formula>IF($M2,IF($N2,TRUE,FALSE),FALSE)</formula>
     </cfRule>
@@ -6584,7 +6584,7 @@
       <formula>IF($M2=TRUE,TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:N3">
+  <conditionalFormatting sqref="A3:I3 K3:N3">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>IF($M3,IF($N3,TRUE,FALSE),FALSE)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Various bug fixes and Issue #100 fix.
</commit_message>
<xml_diff>
--- a/LUMA/tools/spreadsheets/SizingGuide.xlsx
+++ b/LUMA/tools/spreadsheets/SizingGuide.xlsx
@@ -19,12 +19,12 @@
     <sheet name="Desktop" sheetId="7" r:id="rId5"/>
     <sheet name="Laptop" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="72">
   <si>
     <t>No of Nodes</t>
   </si>
@@ -239,15 +239,25 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>Target PPC</t>
+  </si>
+  <si>
+    <t>Actual PPC</t>
+  </si>
+  <si>
+    <t>Error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -329,11 +339,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -366,10 +377,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="14">
     <dxf>
@@ -784,17 +798,18 @@
   <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.21875" bestFit="1" customWidth="1"/>
@@ -850,10 +865,10 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" s="4">
         <v>2</v>
@@ -868,31 +883,31 @@
       </c>
       <c r="F2" s="5">
         <f t="shared" ref="F2:F16" si="2">($C$23/A2)+2</f>
-        <v>194</v>
+        <v>258</v>
       </c>
       <c r="G2" s="5">
         <f t="shared" ref="G2:G16" si="3">($C$24/B2)+2</f>
-        <v>98</v>
+        <v>34</v>
       </c>
       <c r="H2" s="5">
         <f t="shared" ref="H2:H16" si="4">($C$25/C2)+2</f>
-        <v>98</v>
-      </c>
-      <c r="I2" s="5">
+        <v>66</v>
+      </c>
+      <c r="I2" s="4">
         <f>F2*G2*H2</f>
-        <v>1863176</v>
-      </c>
-      <c r="J2" s="5">
+        <v>578952</v>
+      </c>
+      <c r="J2" s="4">
         <f>((F2*G2) + (G2*(H2-2)) + ((F2-2)*(H2-2)))*2</f>
-        <v>93704</v>
-      </c>
-      <c r="K2" s="5">
+        <v>54664</v>
+      </c>
+      <c r="K2" s="4">
         <f t="shared" ref="K2:K16" si="5">J2*E2</f>
-        <v>2248896</v>
+        <v>1311936</v>
       </c>
       <c r="L2" s="5">
         <f t="shared" ref="L2:L16" si="6">K2/$C$26*100</f>
-        <v>5.2955910011574074</v>
+        <v>10.42633056640625</v>
       </c>
       <c r="M2" s="6" t="b">
         <f>IF((F2-FLOOR(F2,1))=0,IF((G2-FLOOR(G2,1))=0,IF((H2-FLOOR(H2,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -923,31 +938,31 @@
       </c>
       <c r="F3" s="5">
         <f t="shared" si="2"/>
-        <v>194</v>
+        <v>130</v>
       </c>
       <c r="G3" s="5">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="H3" s="5">
         <f t="shared" si="4"/>
-        <v>98</v>
-      </c>
-      <c r="I3" s="5">
-        <f t="shared" ref="I2:I16" si="7">F3*G3*H3</f>
-        <v>950600</v>
-      </c>
-      <c r="J3" s="5">
+        <v>66</v>
+      </c>
+      <c r="I3" s="4">
+        <f t="shared" ref="I3:I16" si="7">F3*G3*H3</f>
+        <v>291720</v>
+      </c>
+      <c r="J3" s="4">
         <f t="shared" ref="J3:J16" si="8">((F3*G3) + (G3*(H3-2)) + ((F3-2)*(H3-2)))*2</f>
-        <v>65864</v>
-      </c>
-      <c r="K3" s="5">
+        <v>29576</v>
+      </c>
+      <c r="K3" s="4">
         <f t="shared" si="5"/>
-        <v>3161472</v>
+        <v>1419648</v>
       </c>
       <c r="L3" s="5">
         <f t="shared" si="6"/>
-        <v>7.4444806134259256</v>
+        <v>11.2823486328125</v>
       </c>
       <c r="M3" s="6" t="b">
         <f>IF((F3-FLOOR(F3,1))=0,IF((G3-FLOOR(G3,1))=0,IF((H3-FLOOR(H3,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -978,31 +993,31 @@
       </c>
       <c r="F4" s="5">
         <f t="shared" si="2"/>
-        <v>194</v>
+        <v>130</v>
       </c>
       <c r="G4" s="5">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="H4" s="5">
         <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="I4" s="5">
+        <v>34</v>
+      </c>
+      <c r="I4" s="4">
         <f t="shared" si="7"/>
-        <v>485000</v>
-      </c>
-      <c r="J4" s="5">
+        <v>150280</v>
+      </c>
+      <c r="J4" s="4">
         <f t="shared" si="8"/>
-        <v>42632</v>
-      </c>
-      <c r="K4" s="5">
+        <v>19208</v>
+      </c>
+      <c r="K4" s="4">
         <f t="shared" si="5"/>
-        <v>4092672</v>
+        <v>1843968</v>
       </c>
       <c r="L4" s="5">
         <f t="shared" si="6"/>
-        <v>9.6372251157407405</v>
+        <v>14.654541015625</v>
       </c>
       <c r="M4" s="6" t="b">
         <f t="shared" ref="M4:M6" si="10">IF((F4-FLOOR(F4,1))=0,IF((G4-FLOOR(G4,1))=0,IF((H4-FLOOR(H4,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -1033,31 +1048,31 @@
       </c>
       <c r="F5" s="5">
         <f t="shared" si="2"/>
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="G5" s="5">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="H5" s="5">
         <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="I5" s="5">
+        <v>34</v>
+      </c>
+      <c r="I5" s="4">
         <f t="shared" si="7"/>
-        <v>245000</v>
-      </c>
-      <c r="J5" s="5">
+        <v>76296</v>
+      </c>
+      <c r="J5" s="4">
         <f t="shared" si="8"/>
-        <v>23816</v>
-      </c>
-      <c r="K5" s="5">
+        <v>10760</v>
+      </c>
+      <c r="K5" s="4">
         <f t="shared" si="5"/>
-        <v>4572672</v>
+        <v>2065920</v>
       </c>
       <c r="L5" s="5">
         <f t="shared" si="6"/>
-        <v>10.767505787037036</v>
+        <v>16.41845703125</v>
       </c>
       <c r="M5" s="6" t="b">
         <f t="shared" si="10"/>
@@ -1088,31 +1103,31 @@
       </c>
       <c r="F6" s="5">
         <f t="shared" si="2"/>
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="G6" s="5">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H6" s="5">
         <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="I6" s="5">
+        <v>34</v>
+      </c>
+      <c r="I6" s="4">
         <f t="shared" si="7"/>
-        <v>127400</v>
-      </c>
-      <c r="J6" s="5">
+        <v>40392</v>
+      </c>
+      <c r="J6" s="4">
         <f t="shared" si="8"/>
-        <v>16808</v>
-      </c>
-      <c r="K6" s="5">
+        <v>7624</v>
+      </c>
+      <c r="K6" s="4">
         <f t="shared" si="5"/>
-        <v>6454272</v>
+        <v>2927616</v>
       </c>
       <c r="L6" s="5">
         <f t="shared" si="6"/>
-        <v>15.198206018518517</v>
+        <v>23.2666015625</v>
       </c>
       <c r="M6" s="6" t="b">
         <f t="shared" si="10"/>
@@ -1143,31 +1158,31 @@
       </c>
       <c r="F7" s="5">
         <f t="shared" si="2"/>
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H7" s="5">
         <f t="shared" si="4"/>
-        <v>26</v>
-      </c>
-      <c r="I7" s="5">
+        <v>18</v>
+      </c>
+      <c r="I7" s="4">
         <f t="shared" si="7"/>
-        <v>66248</v>
-      </c>
-      <c r="J7" s="5">
+        <v>21384</v>
+      </c>
+      <c r="J7" s="4">
         <f t="shared" si="8"/>
-        <v>10952</v>
-      </c>
-      <c r="K7" s="5">
+        <v>5000</v>
+      </c>
+      <c r="K7" s="4">
         <f t="shared" si="5"/>
-        <v>8411136</v>
+        <v>3840000</v>
       </c>
       <c r="L7" s="5">
         <f t="shared" si="6"/>
-        <v>19.80613425925926</v>
+        <v>30.517578125</v>
       </c>
       <c r="M7" s="6" t="b">
         <f>IF((F7-FLOOR(F7,1))=0,IF((G7-FLOOR(G7,1))=0,IF((H7-FLOOR(H7,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -1198,31 +1213,31 @@
       </c>
       <c r="F8" s="5">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="G8" s="5">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H8" s="5">
         <f t="shared" si="4"/>
-        <v>26</v>
-      </c>
-      <c r="I8" s="5">
+        <v>18</v>
+      </c>
+      <c r="I8" s="4">
         <f t="shared" si="7"/>
-        <v>33800</v>
-      </c>
-      <c r="J8" s="5">
+        <v>11016</v>
+      </c>
+      <c r="J8" s="4">
         <f t="shared" si="8"/>
-        <v>6152</v>
-      </c>
-      <c r="K8" s="5">
+        <v>2824</v>
+      </c>
+      <c r="K8" s="4">
         <f t="shared" si="5"/>
-        <v>9449472</v>
+        <v>4337664</v>
       </c>
       <c r="L8" s="5">
         <f t="shared" si="6"/>
-        <v>22.251157407407408</v>
+        <v>34.47265625</v>
       </c>
       <c r="M8" s="6" t="b">
         <f t="shared" ref="M8:M16" si="11">IF((F8-FLOOR(F8,1))=0,IF((G8-FLOOR(G8,1))=0,IF((H8-FLOOR(H8,1))=0,TRUE,FALSE),FALSE),FALSE)</f>
@@ -1253,31 +1268,31 @@
       </c>
       <c r="F9" s="5">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H9" s="5">
         <f t="shared" si="4"/>
-        <v>26</v>
-      </c>
-      <c r="I9" s="5">
+        <v>18</v>
+      </c>
+      <c r="I9" s="4">
         <f t="shared" si="7"/>
-        <v>18200</v>
-      </c>
-      <c r="J9" s="5">
+        <v>6120</v>
+      </c>
+      <c r="J9" s="4">
         <f t="shared" si="8"/>
-        <v>4376</v>
-      </c>
-      <c r="K9" s="5">
+        <v>2024</v>
+      </c>
+      <c r="K9" s="4">
         <f t="shared" si="5"/>
-        <v>13443072</v>
+        <v>6217728</v>
       </c>
       <c r="L9" s="5">
         <f t="shared" si="6"/>
-        <v>31.655092592592592</v>
+        <v>49.4140625</v>
       </c>
       <c r="M9" s="6" t="b">
         <f t="shared" si="11"/>
@@ -1308,31 +1323,31 @@
       </c>
       <c r="F10" s="5">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="3"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H10" s="5">
         <f t="shared" si="4"/>
-        <v>14</v>
-      </c>
-      <c r="I10" s="5">
+        <v>10</v>
+      </c>
+      <c r="I10" s="4">
         <f t="shared" si="7"/>
-        <v>9800</v>
-      </c>
-      <c r="J10" s="5">
+        <v>3400</v>
+      </c>
+      <c r="J10" s="4">
         <f t="shared" si="8"/>
-        <v>2888</v>
-      </c>
-      <c r="K10" s="5">
+        <v>1352</v>
+      </c>
+      <c r="K10" s="4">
         <f>J10*E10</f>
-        <v>17743872</v>
+        <v>8306688</v>
       </c>
       <c r="L10" s="5">
         <f t="shared" si="6"/>
-        <v>41.782407407407405</v>
+        <v>66.015625</v>
       </c>
       <c r="M10" s="6" t="b">
         <f t="shared" si="11"/>
@@ -1345,104 +1360,104 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
+        <v>48</v>
+      </c>
+      <c r="B11" s="4">
         <v>16</v>
       </c>
-      <c r="B11" s="4">
-        <v>5</v>
-      </c>
       <c r="C11" s="4">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D11" s="5">
         <f t="shared" si="0"/>
-        <v>6.666666666666667</v>
+        <v>512</v>
       </c>
       <c r="E11" s="5">
         <f t="shared" si="1"/>
-        <v>160</v>
+        <v>12288</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" si="2"/>
-        <v>74</v>
+        <v>18</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="3"/>
-        <v>40.4</v>
+        <v>10</v>
       </c>
       <c r="H11" s="5">
         <f t="shared" si="4"/>
-        <v>98</v>
-      </c>
-      <c r="I11" s="5">
+        <v>10</v>
+      </c>
+      <c r="I11" s="4">
         <f t="shared" si="7"/>
-        <v>292980.8</v>
-      </c>
-      <c r="J11" s="5">
+        <v>1800</v>
+      </c>
+      <c r="J11" s="4">
         <f t="shared" si="8"/>
-        <v>27560</v>
-      </c>
-      <c r="K11" s="5">
+        <v>776</v>
+      </c>
+      <c r="K11" s="4">
         <f t="shared" si="5"/>
-        <v>4409600</v>
+        <v>9535488</v>
       </c>
       <c r="L11" s="5">
         <f t="shared" si="6"/>
-        <v>10.383511766975309</v>
+        <v>75.78125</v>
       </c>
       <c r="M11" s="6" t="b">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N11" s="6" t="b">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="B12" s="4">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C12" s="4">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D12" s="5">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>1024</v>
       </c>
       <c r="E12" s="5">
         <f t="shared" si="1"/>
-        <v>384</v>
+        <v>24576</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" si="2"/>
-        <v>146</v>
+        <v>18</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="H12" s="5">
         <f t="shared" si="4"/>
-        <v>34</v>
-      </c>
-      <c r="I12" s="5">
+        <v>10</v>
+      </c>
+      <c r="I12" s="4">
         <f t="shared" si="7"/>
-        <v>129064</v>
-      </c>
-      <c r="J12" s="5">
+        <v>1080</v>
+      </c>
+      <c r="J12" s="4">
         <f t="shared" si="8"/>
-        <v>18472</v>
-      </c>
-      <c r="K12" s="5">
+        <v>568</v>
+      </c>
+      <c r="K12" s="4">
         <f t="shared" si="5"/>
-        <v>7093248</v>
+        <v>13959168</v>
       </c>
       <c r="L12" s="5">
         <f t="shared" si="6"/>
-        <v>16.702835648148149</v>
+        <v>110.9375</v>
       </c>
       <c r="M12" s="6" t="b">
         <f t="shared" si="11"/>
@@ -1473,31 +1488,31 @@
       </c>
       <c r="F13" s="5">
         <f t="shared" si="2"/>
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="H13" s="5">
         <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="I13" s="5">
+        <v>34</v>
+      </c>
+      <c r="I13" s="4">
         <f t="shared" si="7"/>
-        <v>185000</v>
-      </c>
-      <c r="J13" s="5">
+        <v>57800</v>
+      </c>
+      <c r="J13" s="4">
         <f t="shared" si="8"/>
-        <v>19112</v>
-      </c>
-      <c r="K13" s="5">
+        <v>8648</v>
+      </c>
+      <c r="K13" s="4">
         <f t="shared" si="5"/>
-        <v>4892672</v>
+        <v>2213888</v>
       </c>
       <c r="L13" s="5">
         <f t="shared" si="6"/>
-        <v>11.5210262345679</v>
+        <v>17.594401041666664</v>
       </c>
       <c r="M13" s="6" t="b">
         <f t="shared" si="11"/>
@@ -1528,31 +1543,31 @@
       </c>
       <c r="F14" s="5">
         <f t="shared" si="2"/>
-        <v>146</v>
+        <v>98</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H14" s="5">
         <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="I14" s="5">
+        <v>34</v>
+      </c>
+      <c r="I14" s="4">
         <f t="shared" si="7"/>
-        <v>189800</v>
-      </c>
-      <c r="J14" s="5">
+        <v>59976</v>
+      </c>
+      <c r="J14" s="4">
         <f t="shared" si="8"/>
-        <v>23912</v>
-      </c>
-      <c r="K14" s="5">
+        <v>10824</v>
+      </c>
+      <c r="K14" s="4">
         <f t="shared" si="5"/>
-        <v>6121472</v>
+        <v>2770944</v>
       </c>
       <c r="L14" s="5">
         <f t="shared" si="6"/>
-        <v>14.414544753086419</v>
+        <v>22.021484375</v>
       </c>
       <c r="M14" s="6" t="b">
         <f t="shared" si="11"/>
@@ -1583,31 +1598,31 @@
       </c>
       <c r="F15" s="5">
         <f t="shared" si="2"/>
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="3"/>
-        <v>21.2</v>
+        <v>14.8</v>
       </c>
       <c r="H15" s="5">
         <f t="shared" si="4"/>
-        <v>98</v>
-      </c>
-      <c r="I15" s="5">
+        <v>66</v>
+      </c>
+      <c r="I15" s="4">
         <f t="shared" si="7"/>
-        <v>153742.39999999999</v>
-      </c>
-      <c r="J15" s="5">
+        <v>48840</v>
+      </c>
+      <c r="J15" s="4">
         <f t="shared" si="8"/>
-        <v>21032</v>
-      </c>
-      <c r="K15" s="5">
+        <v>9518.4</v>
+      </c>
+      <c r="K15" s="4">
         <f t="shared" si="5"/>
-        <v>6730240</v>
+        <v>3045888</v>
       </c>
       <c r="L15" s="5">
         <f t="shared" si="6"/>
-        <v>15.848042052469136</v>
+        <v>24.20654296875</v>
       </c>
       <c r="M15" s="6" t="b">
         <f t="shared" si="11"/>
@@ -1638,31 +1653,31 @@
       </c>
       <c r="F16" s="5">
         <f t="shared" si="2"/>
-        <v>117.2</v>
+        <v>78.8</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" si="3"/>
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="I16" s="5">
+        <v>34</v>
+      </c>
+      <c r="I16" s="4">
         <f t="shared" si="7"/>
-        <v>152360</v>
-      </c>
-      <c r="J16" s="5">
+        <v>48225.599999999999</v>
+      </c>
+      <c r="J16" s="4">
         <f t="shared" si="8"/>
-        <v>19649.600000000002</v>
-      </c>
-      <c r="K16" s="5">
+        <v>8904</v>
+      </c>
+      <c r="K16" s="4">
         <f t="shared" si="5"/>
-        <v>6287872.0000000009</v>
+        <v>2849280</v>
       </c>
       <c r="L16" s="5">
         <f t="shared" si="6"/>
-        <v>14.806375385802472</v>
+        <v>22.64404296875</v>
       </c>
       <c r="M16" s="6" t="b">
         <f t="shared" si="11"/>
@@ -1689,7 +1704,7 @@
         <v>68</v>
       </c>
       <c r="B20" s="14">
-        <v>192</v>
+        <v>128</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>18</v>
@@ -1723,10 +1738,14 @@
       <c r="C22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="18"/>
+      <c r="E22" s="20"/>
+      <c r="G22" t="s">
+        <v>70</v>
+      </c>
+      <c r="H22" s="13">
+        <f>I11</f>
+        <v>1800</v>
+      </c>
       <c r="J22" s="17"/>
       <c r="K22" s="18"/>
       <c r="L22" s="17"/>
@@ -1742,12 +1761,15 @@
       </c>
       <c r="C23" s="3">
         <f>CEILING($B$20*B23,1)</f>
-        <v>1152</v>
-      </c>
-      <c r="E23" s="12"/>
+        <v>768</v>
+      </c>
       <c r="F23" s="17"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="19"/>
+      <c r="G23" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" s="3">
+        <v>2937096</v>
+      </c>
       <c r="I23" s="18"/>
       <c r="J23" s="19"/>
       <c r="K23" s="18"/>
@@ -1764,12 +1786,17 @@
       </c>
       <c r="C24" s="3">
         <f t="shared" ref="C24:C25" si="12">CEILING($B$20*B24,1)</f>
-        <v>192</v>
+        <v>128</v>
       </c>
       <c r="E24" s="12"/>
       <c r="F24" s="17"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
+      <c r="G24" t="s">
+        <v>71</v>
+      </c>
+      <c r="H24" s="21">
+        <f>(H22-H23)/H23</f>
+        <v>-0.99938714975608556</v>
+      </c>
       <c r="I24" s="18"/>
       <c r="J24" s="19"/>
       <c r="K24" s="18"/>
@@ -1786,7 +1813,7 @@
       </c>
       <c r="C25" s="3">
         <f t="shared" si="12"/>
-        <v>192</v>
+        <v>128</v>
       </c>
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
@@ -1804,7 +1831,7 @@
       </c>
       <c r="C26" s="3">
         <f>C23*C24*C25</f>
-        <v>42467328</v>
+        <v>12582912</v>
       </c>
       <c r="F26" s="17"/>
       <c r="G26" s="17"/>

</xml_diff>